<commit_message>
Customer search code changes commit
</commit_message>
<xml_diff>
--- a/ULS_Ijarah_MainRepository/TestData/IjarahTestData.xlsx
+++ b/ULS_Ijarah_MainRepository/TestData/IjarahTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600" firstSheet="33" activeTab="37"/>
   </bookViews>
   <sheets>
     <sheet name="ijara_LoginCredentials" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2154" uniqueCount="979">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2154" uniqueCount="980">
   <si>
     <t>UserName</t>
   </si>
@@ -2988,6 +2988,9 @@
   </si>
   <si>
     <t>Monic</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -3750,18 +3753,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3790,6 +3781,18 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -25871,7 +25874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+    <sheetView topLeftCell="S1" workbookViewId="0">
       <selection activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
@@ -27797,9 +27800,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I155"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E151" sqref="E151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -27851,7 +27854,7 @@
       <c r="B2" s="25" t="s">
         <v>308</v>
       </c>
-      <c r="C2" s="121" t="s">
+      <c r="C2" s="132" t="s">
         <v>880</v>
       </c>
       <c r="D2" s="117" t="s">
@@ -27865,7 +27868,7 @@
       <c r="B3" s="25" t="s">
         <v>313</v>
       </c>
-      <c r="C3" s="122"/>
+      <c r="C3" s="133"/>
       <c r="D3" s="117" t="s">
         <v>127</v>
       </c>
@@ -27877,7 +27880,7 @@
       <c r="B4" s="25" t="s">
         <v>319</v>
       </c>
-      <c r="C4" s="122"/>
+      <c r="C4" s="133"/>
       <c r="D4" s="117" t="s">
         <v>127</v>
       </c>
@@ -27889,7 +27892,7 @@
       <c r="B5" s="25" t="s">
         <v>321</v>
       </c>
-      <c r="C5" s="122"/>
+      <c r="C5" s="133"/>
       <c r="D5" s="117" t="s">
         <v>127</v>
       </c>
@@ -27901,7 +27904,7 @@
       <c r="B6" s="25" t="s">
         <v>967</v>
       </c>
-      <c r="C6" s="122"/>
+      <c r="C6" s="133"/>
       <c r="D6" s="117" t="s">
         <v>127</v>
       </c>
@@ -27913,7 +27916,7 @@
       <c r="B7" s="25" t="s">
         <v>968</v>
       </c>
-      <c r="C7" s="122"/>
+      <c r="C7" s="133"/>
       <c r="D7" s="117" t="s">
         <v>127</v>
       </c>
@@ -27925,7 +27928,7 @@
       <c r="B8" s="25" t="s">
         <v>969</v>
       </c>
-      <c r="C8" s="122"/>
+      <c r="C8" s="133"/>
       <c r="D8" s="117" t="s">
         <v>127</v>
       </c>
@@ -27937,7 +27940,7 @@
       <c r="B9" s="25" t="s">
         <v>970</v>
       </c>
-      <c r="C9" s="122"/>
+      <c r="C9" s="133"/>
       <c r="D9" s="117" t="s">
         <v>127</v>
       </c>
@@ -27949,7 +27952,7 @@
       <c r="B10" s="25" t="s">
         <v>971</v>
       </c>
-      <c r="C10" s="122"/>
+      <c r="C10" s="133"/>
       <c r="D10" s="117" t="s">
         <v>127</v>
       </c>
@@ -27961,7 +27964,7 @@
       <c r="B11" s="25" t="s">
         <v>972</v>
       </c>
-      <c r="C11" s="123"/>
+      <c r="C11" s="134"/>
       <c r="D11" s="117" t="s">
         <v>127</v>
       </c>
@@ -27973,7 +27976,7 @@
       <c r="B12" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="C12" s="125" t="s">
+      <c r="C12" s="121" t="s">
         <v>952</v>
       </c>
       <c r="D12" s="117" t="s">
@@ -27987,7 +27990,7 @@
       <c r="B13" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="C13" s="125"/>
+      <c r="C13" s="121"/>
       <c r="D13" s="117" t="s">
         <v>127</v>
       </c>
@@ -27999,7 +28002,7 @@
       <c r="B14" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="C14" s="125"/>
+      <c r="C14" s="121"/>
       <c r="D14" s="117" t="s">
         <v>127</v>
       </c>
@@ -28011,7 +28014,7 @@
       <c r="B15" s="25" t="s">
         <v>178</v>
       </c>
-      <c r="C15" s="126" t="s">
+      <c r="C15" s="122" t="s">
         <v>953</v>
       </c>
       <c r="D15" s="117" t="s">
@@ -28025,7 +28028,7 @@
       <c r="B16" s="25" t="s">
         <v>213</v>
       </c>
-      <c r="C16" s="127"/>
+      <c r="C16" s="123"/>
       <c r="D16" s="117" t="s">
         <v>127</v>
       </c>
@@ -28037,7 +28040,7 @@
       <c r="B17" s="25" t="s">
         <v>217</v>
       </c>
-      <c r="C17" s="127"/>
+      <c r="C17" s="123"/>
       <c r="D17" s="117" t="s">
         <v>127</v>
       </c>
@@ -28049,7 +28052,7 @@
       <c r="B18" s="25" t="s">
         <v>218</v>
       </c>
-      <c r="C18" s="127"/>
+      <c r="C18" s="123"/>
       <c r="D18" s="117" t="s">
         <v>127</v>
       </c>
@@ -28061,7 +28064,7 @@
       <c r="B19" s="25" t="s">
         <v>220</v>
       </c>
-      <c r="C19" s="128"/>
+      <c r="C19" s="124"/>
       <c r="D19" s="117" t="s">
         <v>127</v>
       </c>
@@ -28076,7 +28079,7 @@
       <c r="B20" s="25" t="s">
         <v>230</v>
       </c>
-      <c r="C20" s="126" t="s">
+      <c r="C20" s="122" t="s">
         <v>954</v>
       </c>
       <c r="D20" s="117" t="s">
@@ -28090,7 +28093,7 @@
       <c r="B21" s="25" t="s">
         <v>232</v>
       </c>
-      <c r="C21" s="127"/>
+      <c r="C21" s="123"/>
       <c r="D21" s="117" t="s">
         <v>127</v>
       </c>
@@ -28102,7 +28105,7 @@
       <c r="B22" s="25" t="s">
         <v>234</v>
       </c>
-      <c r="C22" s="127"/>
+      <c r="C22" s="123"/>
       <c r="D22" s="117" t="s">
         <v>127</v>
       </c>
@@ -28114,7 +28117,7 @@
       <c r="B23" s="25" t="s">
         <v>237</v>
       </c>
-      <c r="C23" s="127"/>
+      <c r="C23" s="123"/>
       <c r="D23" s="117" t="s">
         <v>127</v>
       </c>
@@ -28126,7 +28129,7 @@
       <c r="B24" s="25" t="s">
         <v>243</v>
       </c>
-      <c r="C24" s="127"/>
+      <c r="C24" s="123"/>
       <c r="D24" s="117" t="s">
         <v>127</v>
       </c>
@@ -28138,7 +28141,7 @@
       <c r="B25" s="25" t="s">
         <v>239</v>
       </c>
-      <c r="C25" s="128"/>
+      <c r="C25" s="124"/>
       <c r="D25" s="117" t="s">
         <v>127</v>
       </c>
@@ -28150,7 +28153,7 @@
       <c r="B26" s="25" t="s">
         <v>246</v>
       </c>
-      <c r="C26" s="126" t="s">
+      <c r="C26" s="122" t="s">
         <v>955</v>
       </c>
       <c r="D26" s="117" t="s">
@@ -28164,7 +28167,7 @@
       <c r="B27" s="25" t="s">
         <v>248</v>
       </c>
-      <c r="C27" s="127"/>
+      <c r="C27" s="123"/>
       <c r="D27" s="117" t="s">
         <v>127</v>
       </c>
@@ -28176,7 +28179,7 @@
       <c r="B28" s="25" t="s">
         <v>250</v>
       </c>
-      <c r="C28" s="127"/>
+      <c r="C28" s="123"/>
       <c r="D28" s="117" t="s">
         <v>127</v>
       </c>
@@ -28188,7 +28191,7 @@
       <c r="B29" s="25" t="s">
         <v>252</v>
       </c>
-      <c r="C29" s="127"/>
+      <c r="C29" s="123"/>
       <c r="D29" s="117" t="s">
         <v>127</v>
       </c>
@@ -28200,7 +28203,7 @@
       <c r="B30" s="25" t="s">
         <v>255</v>
       </c>
-      <c r="C30" s="127"/>
+      <c r="C30" s="123"/>
       <c r="D30" s="117" t="s">
         <v>127</v>
       </c>
@@ -28212,7 +28215,7 @@
       <c r="B31" s="25" t="s">
         <v>257</v>
       </c>
-      <c r="C31" s="128"/>
+      <c r="C31" s="124"/>
       <c r="D31" s="117" t="s">
         <v>127</v>
       </c>
@@ -28224,7 +28227,7 @@
       <c r="B32" s="25" t="s">
         <v>273</v>
       </c>
-      <c r="C32" s="126" t="s">
+      <c r="C32" s="122" t="s">
         <v>956</v>
       </c>
       <c r="D32" s="117" t="s">
@@ -28238,7 +28241,7 @@
       <c r="B33" s="25" t="s">
         <v>271</v>
       </c>
-      <c r="C33" s="127"/>
+      <c r="C33" s="123"/>
       <c r="D33" s="117" t="s">
         <v>127</v>
       </c>
@@ -28250,7 +28253,7 @@
       <c r="B34" s="25" t="s">
         <v>285</v>
       </c>
-      <c r="C34" s="127"/>
+      <c r="C34" s="123"/>
       <c r="D34" s="117" t="s">
         <v>127</v>
       </c>
@@ -28262,7 +28265,7 @@
       <c r="B35" s="25" t="s">
         <v>288</v>
       </c>
-      <c r="C35" s="127"/>
+      <c r="C35" s="123"/>
       <c r="D35" s="117" t="s">
         <v>127</v>
       </c>
@@ -28274,7 +28277,7 @@
       <c r="B36" s="25" t="s">
         <v>290</v>
       </c>
-      <c r="C36" s="128"/>
+      <c r="C36" s="124"/>
       <c r="D36" s="117" t="s">
         <v>127</v>
       </c>
@@ -28286,7 +28289,7 @@
       <c r="B37" s="25" t="s">
         <v>367</v>
       </c>
-      <c r="C37" s="129" t="s">
+      <c r="C37" s="125" t="s">
         <v>957</v>
       </c>
       <c r="D37" s="117" t="s">
@@ -28300,7 +28303,7 @@
       <c r="B38" s="25" t="s">
         <v>379</v>
       </c>
-      <c r="C38" s="130"/>
+      <c r="C38" s="126"/>
       <c r="D38" s="117" t="s">
         <v>127</v>
       </c>
@@ -28312,7 +28315,7 @@
       <c r="B39" s="25" t="s">
         <v>384</v>
       </c>
-      <c r="C39" s="130"/>
+      <c r="C39" s="126"/>
       <c r="D39" s="117" t="s">
         <v>127</v>
       </c>
@@ -28324,7 +28327,7 @@
       <c r="B40" s="25" t="s">
         <v>389</v>
       </c>
-      <c r="C40" s="130"/>
+      <c r="C40" s="126"/>
       <c r="D40" s="117" t="s">
         <v>127</v>
       </c>
@@ -28336,7 +28339,7 @@
       <c r="B41" s="25" t="s">
         <v>391</v>
       </c>
-      <c r="C41" s="130"/>
+      <c r="C41" s="126"/>
       <c r="D41" s="117" t="s">
         <v>127</v>
       </c>
@@ -28348,7 +28351,7 @@
       <c r="B42" s="25" t="s">
         <v>394</v>
       </c>
-      <c r="C42" s="130"/>
+      <c r="C42" s="126"/>
       <c r="D42" s="117" t="s">
         <v>127</v>
       </c>
@@ -28360,7 +28363,7 @@
       <c r="B43" s="25" t="s">
         <v>398</v>
       </c>
-      <c r="C43" s="130"/>
+      <c r="C43" s="126"/>
       <c r="D43" s="117" t="s">
         <v>127</v>
       </c>
@@ -28372,7 +28375,7 @@
       <c r="B44" s="25" t="s">
         <v>402</v>
       </c>
-      <c r="C44" s="130"/>
+      <c r="C44" s="126"/>
       <c r="D44" s="117" t="s">
         <v>127</v>
       </c>
@@ -28384,7 +28387,7 @@
       <c r="B45" s="25" t="s">
         <v>404</v>
       </c>
-      <c r="C45" s="130"/>
+      <c r="C45" s="126"/>
       <c r="D45" s="117" t="s">
         <v>127</v>
       </c>
@@ -28396,7 +28399,7 @@
       <c r="B46" s="25" t="s">
         <v>406</v>
       </c>
-      <c r="C46" s="130"/>
+      <c r="C46" s="126"/>
       <c r="D46" s="117" t="s">
         <v>127</v>
       </c>
@@ -28408,7 +28411,7 @@
       <c r="B47" s="25" t="s">
         <v>408</v>
       </c>
-      <c r="C47" s="130"/>
+      <c r="C47" s="126"/>
       <c r="D47" s="117" t="s">
         <v>127</v>
       </c>
@@ -28420,7 +28423,7 @@
       <c r="B48" s="25" t="s">
         <v>410</v>
       </c>
-      <c r="C48" s="131"/>
+      <c r="C48" s="127"/>
       <c r="D48" s="117" t="s">
         <v>127</v>
       </c>
@@ -28432,7 +28435,7 @@
       <c r="B49" s="25" t="s">
         <v>617</v>
       </c>
-      <c r="C49" s="129" t="s">
+      <c r="C49" s="125" t="s">
         <v>958</v>
       </c>
       <c r="D49" s="117" t="s">
@@ -28446,7 +28449,7 @@
       <c r="B50" s="25" t="s">
         <v>619</v>
       </c>
-      <c r="C50" s="130"/>
+      <c r="C50" s="126"/>
       <c r="D50" s="117" t="s">
         <v>127</v>
       </c>
@@ -28458,7 +28461,7 @@
       <c r="B51" s="25" t="s">
         <v>622</v>
       </c>
-      <c r="C51" s="131"/>
+      <c r="C51" s="127"/>
       <c r="D51" s="117" t="s">
         <v>127</v>
       </c>
@@ -28470,7 +28473,7 @@
       <c r="B52" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="C52" s="126" t="s">
+      <c r="C52" s="122" t="s">
         <v>959</v>
       </c>
       <c r="D52" s="117" t="s">
@@ -28484,7 +28487,7 @@
       <c r="B53" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="C53" s="127"/>
+      <c r="C53" s="123"/>
       <c r="D53" s="117" t="s">
         <v>127</v>
       </c>
@@ -28496,7 +28499,7 @@
       <c r="B54" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="C54" s="127"/>
+      <c r="C54" s="123"/>
       <c r="D54" s="117" t="s">
         <v>127</v>
       </c>
@@ -28508,7 +28511,7 @@
       <c r="B55" s="25" t="s">
         <v>879</v>
       </c>
-      <c r="C55" s="127"/>
+      <c r="C55" s="123"/>
       <c r="D55" s="117" t="s">
         <v>127</v>
       </c>
@@ -28520,7 +28523,7 @@
       <c r="B56" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="C56" s="127"/>
+      <c r="C56" s="123"/>
       <c r="D56" s="117" t="s">
         <v>127</v>
       </c>
@@ -28532,7 +28535,7 @@
       <c r="B57" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="C57" s="128"/>
+      <c r="C57" s="124"/>
       <c r="D57" s="117" t="s">
         <v>127</v>
       </c>
@@ -28544,7 +28547,7 @@
       <c r="B58" s="25" t="s">
         <v>428</v>
       </c>
-      <c r="C58" s="132" t="s">
+      <c r="C58" s="128" t="s">
         <v>960</v>
       </c>
       <c r="D58" s="117" t="s">
@@ -28558,7 +28561,7 @@
       <c r="B59" s="25" t="s">
         <v>430</v>
       </c>
-      <c r="C59" s="133"/>
+      <c r="C59" s="129"/>
       <c r="D59" s="117" t="s">
         <v>127</v>
       </c>
@@ -28570,7 +28573,7 @@
       <c r="B60" s="25" t="s">
         <v>438</v>
       </c>
-      <c r="C60" s="133"/>
+      <c r="C60" s="129"/>
       <c r="D60" s="117" t="s">
         <v>127</v>
       </c>
@@ -28582,7 +28585,7 @@
       <c r="B61" s="25" t="s">
         <v>446</v>
       </c>
-      <c r="C61" s="133"/>
+      <c r="C61" s="129"/>
       <c r="D61" s="117" t="s">
         <v>127</v>
       </c>
@@ -28594,7 +28597,7 @@
       <c r="B62" s="25" t="s">
         <v>449</v>
       </c>
-      <c r="C62" s="133"/>
+      <c r="C62" s="129"/>
       <c r="D62" s="117" t="s">
         <v>127</v>
       </c>
@@ -28606,7 +28609,7 @@
       <c r="B63" s="25" t="s">
         <v>452</v>
       </c>
-      <c r="C63" s="133"/>
+      <c r="C63" s="129"/>
       <c r="D63" s="117" t="s">
         <v>127</v>
       </c>
@@ -28618,7 +28621,7 @@
       <c r="B64" s="25" t="s">
         <v>454</v>
       </c>
-      <c r="C64" s="133"/>
+      <c r="C64" s="129"/>
       <c r="D64" s="117" t="s">
         <v>127</v>
       </c>
@@ -28630,7 +28633,7 @@
       <c r="B65" s="25" t="s">
         <v>458</v>
       </c>
-      <c r="C65" s="134"/>
+      <c r="C65" s="130"/>
       <c r="D65" s="117" t="s">
         <v>127</v>
       </c>
@@ -28642,7 +28645,7 @@
       <c r="B66" s="25" t="s">
         <v>895</v>
       </c>
-      <c r="C66" s="124" t="s">
+      <c r="C66" s="131" t="s">
         <v>884</v>
       </c>
       <c r="D66" s="117" t="s">
@@ -28656,7 +28659,7 @@
       <c r="B67" s="25" t="s">
         <v>896</v>
       </c>
-      <c r="C67" s="124"/>
+      <c r="C67" s="131"/>
       <c r="D67" s="117" t="s">
         <v>127</v>
       </c>
@@ -28782,7 +28785,7 @@
       <c r="B77" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="C77" s="124" t="s">
+      <c r="C77" s="131" t="s">
         <v>886</v>
       </c>
       <c r="D77" s="117" t="s">
@@ -28796,7 +28799,7 @@
       <c r="B78" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="C78" s="124"/>
+      <c r="C78" s="131"/>
       <c r="D78" s="117" t="s">
         <v>127</v>
       </c>
@@ -28822,7 +28825,7 @@
       <c r="B80" s="25" t="s">
         <v>532</v>
       </c>
-      <c r="C80" s="124" t="s">
+      <c r="C80" s="131" t="s">
         <v>888</v>
       </c>
       <c r="D80" s="117" t="s">
@@ -28836,7 +28839,7 @@
       <c r="B81" s="25" t="s">
         <v>534</v>
       </c>
-      <c r="C81" s="124"/>
+      <c r="C81" s="131"/>
       <c r="D81" s="117" t="s">
         <v>127</v>
       </c>
@@ -28848,7 +28851,7 @@
       <c r="B82" s="25" t="s">
         <v>537</v>
       </c>
-      <c r="C82" s="124"/>
+      <c r="C82" s="131"/>
       <c r="D82" s="117" t="s">
         <v>127</v>
       </c>
@@ -28860,7 +28863,7 @@
       <c r="B83" s="25" t="s">
         <v>740</v>
       </c>
-      <c r="C83" s="124" t="s">
+      <c r="C83" s="131" t="s">
         <v>889</v>
       </c>
       <c r="D83" s="117" t="s">
@@ -28874,7 +28877,7 @@
       <c r="B84" s="25" t="s">
         <v>747</v>
       </c>
-      <c r="C84" s="124"/>
+      <c r="C84" s="131"/>
       <c r="D84" s="117" t="s">
         <v>127</v>
       </c>
@@ -28886,7 +28889,7 @@
       <c r="B85" s="25" t="s">
         <v>749</v>
       </c>
-      <c r="C85" s="124"/>
+      <c r="C85" s="131"/>
       <c r="D85" s="117" t="s">
         <v>127</v>
       </c>
@@ -28898,7 +28901,7 @@
       <c r="B86" s="25" t="s">
         <v>751</v>
       </c>
-      <c r="C86" s="124"/>
+      <c r="C86" s="131"/>
       <c r="D86" s="117" t="s">
         <v>127</v>
       </c>
@@ -28910,7 +28913,7 @@
       <c r="B87" s="25" t="s">
         <v>753</v>
       </c>
-      <c r="C87" s="124"/>
+      <c r="C87" s="131"/>
       <c r="D87" s="117" t="s">
         <v>127</v>
       </c>
@@ -28922,7 +28925,7 @@
       <c r="B88" s="25" t="s">
         <v>723</v>
       </c>
-      <c r="C88" s="124" t="s">
+      <c r="C88" s="131" t="s">
         <v>890</v>
       </c>
       <c r="D88" s="117" t="s">
@@ -28936,7 +28939,7 @@
       <c r="B89" s="25" t="s">
         <v>725</v>
       </c>
-      <c r="C89" s="124"/>
+      <c r="C89" s="131"/>
       <c r="D89" s="117" t="s">
         <v>127</v>
       </c>
@@ -29102,7 +29105,7 @@
       </c>
       <c r="C102" s="120"/>
       <c r="D102" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -29114,7 +29117,7 @@
       </c>
       <c r="C103" s="120"/>
       <c r="D103" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -29126,7 +29129,7 @@
       </c>
       <c r="C104" s="120"/>
       <c r="D104" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -29138,7 +29141,7 @@
       </c>
       <c r="C105" s="120"/>
       <c r="D105" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -29150,7 +29153,7 @@
       </c>
       <c r="C106" s="120"/>
       <c r="D106" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -29164,7 +29167,7 @@
         <v>909</v>
       </c>
       <c r="D107" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -29176,7 +29179,7 @@
       </c>
       <c r="C108" s="120"/>
       <c r="D108" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -29188,7 +29191,7 @@
       </c>
       <c r="C109" s="120"/>
       <c r="D109" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -29202,7 +29205,7 @@
         <v>910</v>
       </c>
       <c r="D110" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -29214,7 +29217,7 @@
       </c>
       <c r="C111" s="120"/>
       <c r="D111" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -29226,7 +29229,7 @@
       </c>
       <c r="C112" s="120"/>
       <c r="D112" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -29240,7 +29243,7 @@
         <v>923</v>
       </c>
       <c r="D113" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -29252,7 +29255,7 @@
       </c>
       <c r="C114" s="120"/>
       <c r="D114" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -29264,7 +29267,7 @@
       </c>
       <c r="C115" s="120"/>
       <c r="D115" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -29276,7 +29279,7 @@
       </c>
       <c r="C116" s="120"/>
       <c r="D116" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -29288,7 +29291,7 @@
       </c>
       <c r="C117" s="120"/>
       <c r="D117" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -29300,7 +29303,7 @@
       </c>
       <c r="C118" s="120"/>
       <c r="D118" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -29314,7 +29317,7 @@
         <v>924</v>
       </c>
       <c r="D119" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -29326,7 +29329,7 @@
       </c>
       <c r="C120" s="120"/>
       <c r="D120" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -29338,7 +29341,7 @@
       </c>
       <c r="C121" s="120"/>
       <c r="D121" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -29350,7 +29353,7 @@
       </c>
       <c r="C122" s="120"/>
       <c r="D122" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -29364,7 +29367,7 @@
         <v>931</v>
       </c>
       <c r="D123" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -29376,7 +29379,7 @@
       </c>
       <c r="C124" s="120"/>
       <c r="D124" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -29388,7 +29391,7 @@
       </c>
       <c r="C125" s="120"/>
       <c r="D125" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -29400,7 +29403,7 @@
       </c>
       <c r="C126" s="120"/>
       <c r="D126" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -29414,7 +29417,7 @@
         <v>932</v>
       </c>
       <c r="D127" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -29426,7 +29429,7 @@
       </c>
       <c r="C128" s="120"/>
       <c r="D128" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -29438,7 +29441,7 @@
       </c>
       <c r="C129" s="120"/>
       <c r="D129" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -29450,7 +29453,7 @@
       </c>
       <c r="C130" s="120"/>
       <c r="D130" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -29462,7 +29465,7 @@
       </c>
       <c r="C131" s="120"/>
       <c r="D131" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -29474,7 +29477,7 @@
       </c>
       <c r="C132" s="120"/>
       <c r="D132" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -29488,7 +29491,7 @@
         <v>935</v>
       </c>
       <c r="D133" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -29500,7 +29503,7 @@
       </c>
       <c r="C134" s="120"/>
       <c r="D134" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -29512,7 +29515,7 @@
       </c>
       <c r="C135" s="120"/>
       <c r="D135" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -29524,7 +29527,7 @@
       </c>
       <c r="C136" s="120"/>
       <c r="D136" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -29536,7 +29539,7 @@
       </c>
       <c r="C137" s="120"/>
       <c r="D137" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -29548,7 +29551,7 @@
       </c>
       <c r="C138" s="120"/>
       <c r="D138" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -29562,7 +29565,7 @@
         <v>950</v>
       </c>
       <c r="D139" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -29574,7 +29577,7 @@
       </c>
       <c r="C140" s="120"/>
       <c r="D140" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -29586,7 +29589,7 @@
       </c>
       <c r="C141" s="120"/>
       <c r="D141" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -29598,7 +29601,7 @@
       </c>
       <c r="C142" s="120"/>
       <c r="D142" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -29610,7 +29613,7 @@
       </c>
       <c r="C143" s="120"/>
       <c r="D143" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -29622,7 +29625,7 @@
       </c>
       <c r="C144" s="120"/>
       <c r="D144" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -29634,7 +29637,7 @@
       </c>
       <c r="C145" s="120"/>
       <c r="D145" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -29646,7 +29649,7 @@
       </c>
       <c r="C146" s="120"/>
       <c r="D146" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -29658,7 +29661,7 @@
       </c>
       <c r="C147" s="120"/>
       <c r="D147" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -29670,7 +29673,7 @@
       </c>
       <c r="C148" s="120"/>
       <c r="D148" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -29682,7 +29685,7 @@
       </c>
       <c r="C149" s="120"/>
       <c r="D149" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -29694,7 +29697,7 @@
       </c>
       <c r="C150" s="120"/>
       <c r="D150" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -29706,7 +29709,7 @@
       </c>
       <c r="C151" s="120"/>
       <c r="D151" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -29718,7 +29721,7 @@
       </c>
       <c r="C152" s="120"/>
       <c r="D152" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -29732,7 +29735,7 @@
         <v>951</v>
       </c>
       <c r="D153" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -29744,7 +29747,7 @@
       </c>
       <c r="C154" s="120"/>
       <c r="D154" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -29756,24 +29759,11 @@
       </c>
       <c r="C155" s="120"/>
       <c r="D155" s="117" t="s">
-        <v>127</v>
+        <v>979</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="C90:C93"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="C15:C19"/>
-    <mergeCell ref="C20:C25"/>
-    <mergeCell ref="C26:C31"/>
-    <mergeCell ref="C32:C36"/>
-    <mergeCell ref="C37:C48"/>
-    <mergeCell ref="C49:C51"/>
-    <mergeCell ref="C52:C57"/>
-    <mergeCell ref="C58:C65"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="C68:C70"/>
-    <mergeCell ref="C71:C75"/>
     <mergeCell ref="C153:C155"/>
     <mergeCell ref="C2:C11"/>
     <mergeCell ref="C119:C122"/>
@@ -29790,6 +29780,19 @@
     <mergeCell ref="C80:C82"/>
     <mergeCell ref="C83:C87"/>
     <mergeCell ref="C88:C89"/>
+    <mergeCell ref="C90:C93"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="C15:C19"/>
+    <mergeCell ref="C20:C25"/>
+    <mergeCell ref="C26:C31"/>
+    <mergeCell ref="C32:C36"/>
+    <mergeCell ref="C37:C48"/>
+    <mergeCell ref="C49:C51"/>
+    <mergeCell ref="C52:C57"/>
+    <mergeCell ref="C58:C65"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="C68:C70"/>
+    <mergeCell ref="C71:C75"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:B1048576 C1:C2 C12:C1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="4"/>

</xml_diff>

<commit_message>
Ijarah - customer debt, Application details scripts are updated
</commit_message>
<xml_diff>
--- a/ULS_Ijarah_MainRepository/TestData/IjarahTestData.xlsx
+++ b/ULS_Ijarah_MainRepository/TestData/IjarahTestData.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2158" uniqueCount="982">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2157" uniqueCount="981">
   <si>
     <t>UserName</t>
   </si>
@@ -2984,19 +2984,16 @@
     <t>No</t>
   </si>
   <si>
-    <t>3082</t>
-  </si>
-  <si>
     <t>UserReturn</t>
   </si>
   <si>
-    <t>0345</t>
-  </si>
-  <si>
     <t>01069</t>
   </si>
   <si>
     <t>0362</t>
+  </si>
+  <si>
+    <t>0365</t>
   </si>
 </sst>
 </file>
@@ -3761,6 +3758,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3789,18 +3798,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4159,16 +4156,16 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="19.33203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="10.49609375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="15.109375" collapsed="true"/>
-    <col min="4" max="4" style="3" width="9.109375" collapsed="false"/>
-    <col min="5" max="16384" style="3" width="9.109375" collapsed="true"/>
+    <col min="1" max="1" width="19.33203125" style="3" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.44140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.109375" style="3"/>
+    <col min="5" max="16384" width="9.109375" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -4184,10 +4181,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="120" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="B2" s="120" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="C2" s="121" t="s">
         <v>6</v>
@@ -4287,7 +4284,7 @@
         <v>625</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>6</v>
@@ -4353,7 +4350,7 @@
         <v>850</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>977</v>
+        <v>980</v>
       </c>
       <c r="C17" s="83" t="s">
         <v>6</v>
@@ -4391,34 +4388,34 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="17.6640625" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" style="3" width="26.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="3" width="21.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="20.44140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="3" width="32.33203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="3" width="23.109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="3" width="25.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="3" width="27.109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="3" width="26.33203125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="3" width="18.6640625" collapsed="true"/>
-    <col min="12" max="12" style="3" width="9.109375" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="3" width="29.5546875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" style="3" width="14.88671875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" style="3" width="19.44140625" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" style="3" width="20.88671875" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" style="3" width="30.6640625" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" style="3" width="21.88671875" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" style="3" width="41.5546875" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" style="3" width="24.44140625" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" style="3" width="29.5546875" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" style="3" width="24.109375" collapsed="true"/>
-    <col min="23" max="24" customWidth="true" style="3" width="26.88671875" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" style="3" width="26.44140625" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" style="3" width="22.5546875" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" style="3" width="17.88671875" collapsed="true"/>
-    <col min="28" max="28" customWidth="true" style="3" width="16.109375" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" style="3" width="20.44140625" collapsed="true"/>
-    <col min="30" max="16384" style="3" width="9.109375" collapsed="true"/>
+    <col min="1" max="1" width="17.6640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="26" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21" style="3" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.44140625" style="3" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="32.33203125" style="3" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="23.109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="25" style="3" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="27.109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="26.33203125" style="3" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.6640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="9.109375" style="3" collapsed="1"/>
+    <col min="13" max="13" width="29.5546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="14.88671875" style="3" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="19.44140625" style="3" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="20.88671875" style="3" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="30.6640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="21.88671875" style="3" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="41.5546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="24.44140625" style="3" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="29.5546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="24.109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="23" max="24" width="26.88671875" style="3" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="26.44140625" style="3" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="22.5546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="17.88671875" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="16.109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="20.44140625" style="3" customWidth="1" collapsed="1"/>
+    <col min="30" max="16384" width="9.109375" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
@@ -4820,9 +4817,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="22.5546875" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="22.33203125" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="18.88671875" collapsed="false"/>
+    <col min="1" max="1" width="22.5546875" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="42" thickBot="1">
@@ -5189,12 +5186,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="51.6640625" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="25.6640625" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="31.0" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="34.5546875" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="29.0" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="17.88671875" collapsed="false"/>
+    <col min="1" max="1" width="51.6640625" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="3" max="3" width="31" customWidth="1"/>
+    <col min="4" max="4" width="34.5546875" customWidth="1"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -6267,11 +6264,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.5546875" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="17.0" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="14.109375" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="17.44140625" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="16.0" collapsed="false"/>
+    <col min="1" max="1" width="14.5546875" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -6349,19 +6346,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.33203125" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="20.33203125" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" style="3" width="9.5546875" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" style="3" width="13.33203125" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" style="3" width="12.88671875" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" style="3" width="15.44140625" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" style="3" width="14.5546875" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" style="3" width="16.0" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" width="15.109375" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="17.6640625" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" width="19.33203125" collapsed="false"/>
-    <col min="12" max="12" customWidth="true" width="16.44140625" collapsed="false"/>
-    <col min="13" max="13" customWidth="true" width="14.33203125" collapsed="false"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="16" style="3" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" customWidth="1"/>
+    <col min="10" max="10" width="17.6640625" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" customWidth="1"/>
+    <col min="12" max="12" width="16.44140625" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -6590,16 +6587,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="12.44140625" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="18.109375" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="12.33203125" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="18.44140625" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="13.109375" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="17.0" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="18.88671875" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="13.88671875" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" width="20.88671875" collapsed="false"/>
-    <col min="12" max="12" customWidth="true" width="22.6640625" collapsed="false"/>
+    <col min="1" max="1" width="12.44140625" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="7" max="7" width="18.88671875" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" customWidth="1"/>
+    <col min="11" max="11" width="20.88671875" customWidth="1"/>
+    <col min="12" max="12" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
@@ -6833,13 +6830,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="26.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="24.5546875" collapsed="true"/>
-    <col min="3" max="34" customWidth="true" style="3" width="33.88671875" collapsed="true"/>
-    <col min="35" max="35" customWidth="true" style="3" width="26.33203125" collapsed="true"/>
-    <col min="36" max="36" customWidth="true" style="3" width="30.44140625" collapsed="true"/>
-    <col min="37" max="37" customWidth="true" style="3" width="22.6640625" collapsed="true"/>
-    <col min="38" max="16384" style="3" width="9.109375" collapsed="true"/>
+    <col min="1" max="1" width="26.33203125" style="3" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.5546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="3" max="34" width="33.88671875" style="3" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="26.33203125" style="3" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="30.44140625" style="3" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="22.6640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="38" max="16384" width="9.109375" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34">
@@ -7112,17 +7109,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.5546875" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="16.109375" collapsed="false"/>
-    <col min="3" max="4" customWidth="true" width="20.5546875" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="11.88671875" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="13.109375" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="13.33203125" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="27.33203125" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" width="22.109375" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="14.33203125" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" width="14.5546875" collapsed="false"/>
-    <col min="13" max="14" customWidth="true" width="9.109375" collapsed="false"/>
+    <col min="1" max="1" width="17.5546875" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" customWidth="1"/>
+    <col min="3" max="4" width="20.5546875" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="8" max="8" width="27.33203125" customWidth="1"/>
+    <col min="9" max="9" width="22.109375" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" customWidth="1"/>
+    <col min="11" max="11" width="14.5546875" customWidth="1"/>
+    <col min="13" max="14" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25">
@@ -7230,16 +7227,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="12.88671875" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="17.6640625" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="22.88671875" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="25.109375" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="29.44140625" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="24.5546875" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="19.109375" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="17.5546875" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" width="18.33203125" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="22.0" collapsed="false"/>
+    <col min="1" max="1" width="12.88671875" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.88671875" customWidth="1"/>
+    <col min="4" max="4" width="25.109375" customWidth="1"/>
+    <col min="5" max="5" width="29.44140625" customWidth="1"/>
+    <col min="6" max="6" width="24.5546875" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -7373,20 +7370,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="18.109375" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" style="3" width="23.6640625" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" style="3" width="9.5546875" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" style="3" width="24.33203125" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" style="3" width="23.6640625" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" style="3" width="15.6640625" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" style="3" width="15.5546875" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" style="3" width="14.88671875" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" style="3" width="26.33203125" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" style="3" width="13.5546875" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" style="3" width="19.33203125" collapsed="false"/>
-    <col min="12" max="12" customWidth="true" style="3" width="24.6640625" collapsed="false"/>
-    <col min="13" max="13" customWidth="true" style="3" width="20.5546875" collapsed="false"/>
-    <col min="14" max="16384" style="3" width="8.88671875" collapsed="false"/>
+    <col min="1" max="1" width="18.109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="14.88671875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="26.33203125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="24.6640625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="20.5546875" style="3" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="94" customFormat="1">
@@ -7572,21 +7569,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="21.6640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.6640625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="14.5546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="16.44140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="16.5546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="30.5546875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="32.6640625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="26.109375" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="17.5546875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="13.6640625" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="38.0" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="16.33203125" collapsed="true"/>
+    <col min="1" max="1" width="16.109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.5546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.44140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.5546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="30.5546875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="32.6640625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="26.109375" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.5546875" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="13.6640625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="38" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="16.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1">
@@ -7796,7 +7793,7 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC7"/>
+  <dimension ref="A1:AMJ7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B7"/>
@@ -7804,35 +7801,35 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.6640625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="92" width="18.88671875" collapsed="false"/>
-    <col min="2" max="3" customWidth="true" style="92" width="27.6640625" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" style="92" width="22.33203125" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" style="92" width="21.6640625" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" style="92" width="34.33203125" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" style="92" width="24.5546875" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" style="92" width="26.5546875" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" style="92" width="28.88671875" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" style="92" width="28.0" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" style="92" width="19.88671875" collapsed="false"/>
-    <col min="12" max="12" customWidth="true" style="92" width="9.6640625" collapsed="false"/>
-    <col min="13" max="13" customWidth="true" style="92" width="31.44140625" collapsed="false"/>
-    <col min="14" max="14" customWidth="true" style="92" width="15.6640625" collapsed="false"/>
-    <col min="15" max="15" customWidth="true" style="92" width="20.5546875" collapsed="false"/>
-    <col min="16" max="16" customWidth="true" style="92" width="22.109375" collapsed="false"/>
-    <col min="17" max="17" customWidth="true" style="92" width="32.6640625" collapsed="false"/>
-    <col min="18" max="18" customWidth="true" style="92" width="23.33203125" collapsed="false"/>
-    <col min="19" max="19" customWidth="true" style="92" width="44.33203125" collapsed="false"/>
-    <col min="20" max="20" customWidth="true" style="92" width="26.0" collapsed="false"/>
-    <col min="21" max="21" customWidth="true" style="92" width="31.44140625" collapsed="false"/>
-    <col min="22" max="22" customWidth="true" style="92" width="25.6640625" collapsed="false"/>
-    <col min="23" max="24" customWidth="true" style="92" width="28.5546875" collapsed="false"/>
-    <col min="25" max="25" customWidth="true" style="92" width="28.109375" collapsed="false"/>
-    <col min="26" max="26" customWidth="true" style="92" width="24.0" collapsed="false"/>
-    <col min="27" max="27" customWidth="true" style="92" width="19.0" collapsed="false"/>
-    <col min="28" max="28" customWidth="true" style="92" width="17.109375" collapsed="false"/>
-    <col min="29" max="29" customWidth="true" style="92" width="21.6640625" collapsed="false"/>
-    <col min="30" max="1024" customWidth="true" style="87" width="9.6640625" collapsed="false"/>
-    <col min="1025" max="16384" style="74" width="20.6640625" collapsed="false"/>
+    <col min="1" max="1" width="18.88671875" style="92" customWidth="1"/>
+    <col min="2" max="3" width="27.6640625" style="92" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" style="92" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" style="92" customWidth="1"/>
+    <col min="6" max="6" width="34.33203125" style="92" customWidth="1"/>
+    <col min="7" max="7" width="24.5546875" style="92" customWidth="1"/>
+    <col min="8" max="8" width="26.5546875" style="92" customWidth="1"/>
+    <col min="9" max="9" width="28.88671875" style="92" customWidth="1"/>
+    <col min="10" max="10" width="28" style="92" customWidth="1"/>
+    <col min="11" max="11" width="19.88671875" style="92" customWidth="1"/>
+    <col min="12" max="12" width="9.6640625" style="92" customWidth="1"/>
+    <col min="13" max="13" width="31.44140625" style="92" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" style="92" customWidth="1"/>
+    <col min="15" max="15" width="20.5546875" style="92" customWidth="1"/>
+    <col min="16" max="16" width="22.109375" style="92" customWidth="1"/>
+    <col min="17" max="17" width="32.6640625" style="92" customWidth="1"/>
+    <col min="18" max="18" width="23.33203125" style="92" customWidth="1"/>
+    <col min="19" max="19" width="44.33203125" style="92" customWidth="1"/>
+    <col min="20" max="20" width="26" style="92" customWidth="1"/>
+    <col min="21" max="21" width="31.44140625" style="92" customWidth="1"/>
+    <col min="22" max="22" width="25.6640625" style="92" customWidth="1"/>
+    <col min="23" max="24" width="28.5546875" style="92" customWidth="1"/>
+    <col min="25" max="25" width="28.109375" style="92" customWidth="1"/>
+    <col min="26" max="26" width="24" style="92" customWidth="1"/>
+    <col min="27" max="27" width="19" style="92" customWidth="1"/>
+    <col min="28" max="28" width="17.109375" style="92" customWidth="1"/>
+    <col min="29" max="29" width="21.6640625" style="92" customWidth="1"/>
+    <col min="30" max="1024" width="9.6640625" style="87" customWidth="1"/>
+    <col min="1025" max="16384" width="20.6640625" style="74"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
@@ -8206,31 +8203,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.88671875" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.44140625" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.0" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.5546875" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="16.109375" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.6640625" collapsed="false"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.5546875" collapsed="false"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="18.33203125" collapsed="false"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="11.44140625" collapsed="false"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="20.33203125" collapsed="false"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="15.88671875" collapsed="false"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="15.109375" collapsed="false"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="26.88671875" collapsed="false"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="14.88671875" collapsed="false"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="16.6640625" collapsed="false"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="27.109375" collapsed="false"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="20.6640625" collapsed="false"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="23.0" collapsed="false"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="7.5546875" collapsed="false"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="8.109375" collapsed="false"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="6.88671875" collapsed="false"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="12.6640625" collapsed="false"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="18.44140625" collapsed="false"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="10.33203125" collapsed="false"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="11.6640625" collapsed="false"/>
+    <col min="1" max="1" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16384" s="11" customFormat="1">
@@ -24941,7 +24938,7 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:AMJ7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B4"/>
@@ -24949,13 +24946,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="73" width="20.109375" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" style="73" width="20.44140625" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" style="73" width="20.6640625" collapsed="false"/>
-    <col min="4" max="10" customWidth="true" style="73" width="9.109375" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" style="73" width="15.109375" collapsed="false"/>
-    <col min="12" max="1024" customWidth="true" style="72" width="9.109375" collapsed="false"/>
-    <col min="1025" max="16384" style="74" width="20.5546875" collapsed="false"/>
+    <col min="1" max="1" width="20.109375" style="73" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" style="73" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" style="73" customWidth="1"/>
+    <col min="4" max="10" width="9.109375" style="73" customWidth="1"/>
+    <col min="11" max="11" width="15.109375" style="73" customWidth="1"/>
+    <col min="12" max="1024" width="9.109375" style="72" customWidth="1"/>
+    <col min="1025" max="16384" width="20.5546875" style="74"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -25121,9 +25118,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.109375" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="21.109375" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="17.6640625" collapsed="false"/>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -25210,7 +25207,7 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:AMJ4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B4"/>
@@ -25218,10 +25215,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.33203125" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="81" width="16.0" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" style="81" width="19.0" collapsed="false"/>
-    <col min="3" max="1024" customWidth="true" style="81" width="16.0" collapsed="false"/>
-    <col min="1025" max="16384" style="85" width="10.33203125" collapsed="false"/>
+    <col min="1" max="1" width="16" style="81" customWidth="1"/>
+    <col min="2" max="2" width="19" style="81" customWidth="1"/>
+    <col min="3" max="1024" width="16" style="81" customWidth="1"/>
+    <col min="1025" max="16384" width="10.33203125" style="85"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -25285,9 +25282,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.88671875" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.33203125" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="7.0" collapsed="false"/>
+    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -25349,9 +25346,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.5546875" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="16.88671875" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="22.109375" collapsed="false"/>
+    <col min="1" max="1" width="17.5546875" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -25425,20 +25422,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="14.44140625" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" style="3" width="23.109375" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" style="3" width="13.109375" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" style="3" width="17.33203125" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" style="3" width="18.88671875" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" style="3" width="16.0" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" style="3" width="11.33203125" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" style="3" width="10.33203125" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" style="3" width="16.88671875" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" style="3" width="12.6640625" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" style="3" width="12.33203125" collapsed="false"/>
-    <col min="12" max="12" customWidth="true" style="3" width="17.6640625" collapsed="false"/>
-    <col min="13" max="13" customWidth="true" style="3" width="18.109375" collapsed="false"/>
-    <col min="14" max="16384" style="3" width="8.88671875" collapsed="false"/>
+    <col min="1" max="1" width="14.44140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="18.88671875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="16" style="3" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="16.88671875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="18.109375" style="3" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -25645,9 +25642,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.6640625" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="18.5546875" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="17.5546875" collapsed="false"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -25742,11 +25739,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.109375" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.44140625" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="12.88671875" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="22.33203125" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="21.44140625" collapsed="false"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="101" customFormat="1">
@@ -25901,38 +25898,38 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="20.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="35.5546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="30.88671875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="3" width="25.6640625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="24.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="3" width="30.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="3" width="40.6640625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="3" width="27.5546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="3" width="32.5546875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="3" width="43.33203125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="3" width="32.109375" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="3" width="30.88671875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="3" width="28.88671875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" style="3" width="32.109375" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" style="3" width="21.33203125" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" style="3" width="39.6640625" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" style="3" width="15.5546875" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" style="3" width="40.88671875" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" style="3" width="24.0" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" style="3" width="31.109375" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" style="3" width="31.33203125" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" style="3" width="15.109375" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" style="3" width="16.6640625" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" style="3" width="19.44140625" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" style="3" width="20.6640625" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" style="3" width="24.0" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" style="3" width="31.44140625" collapsed="true"/>
-    <col min="28" max="28" customWidth="true" style="3" width="26.6640625" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" style="3" width="19.5546875" collapsed="true"/>
-    <col min="30" max="30" customWidth="true" style="3" width="26.44140625" collapsed="true"/>
-    <col min="31" max="31" customWidth="true" style="3" width="17.5546875" collapsed="true"/>
-    <col min="32" max="16384" style="3" width="9.109375" collapsed="true"/>
+    <col min="1" max="1" width="20.6640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.5546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="30.88671875" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.6640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24" style="3" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30" style="3" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="40.6640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="27.5546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="32.5546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="43.33203125" style="3" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="32.109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="30.88671875" style="3" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="28.88671875" style="3" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="32.109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="21.33203125" style="3" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="39.6640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="15.5546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="40.88671875" style="3" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="24" style="3" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="31.109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="31.33203125" style="3" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="15.109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="16.6640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="19.44140625" style="3" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="20.6640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="24" style="3" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="31.44140625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="26.6640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="19.5546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="26.44140625" style="3" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="17.5546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="32" max="16384" width="9.109375" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
@@ -26226,7 +26223,7 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:AMJ7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:B6"/>
@@ -26234,10 +26231,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="43.6640625" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="72" width="18.109375" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" style="72" width="43.6640625" collapsed="false"/>
-    <col min="3" max="1024" customWidth="true" style="72" width="12.109375" collapsed="false"/>
-    <col min="1025" max="16384" style="74" width="43.6640625" collapsed="false"/>
+    <col min="1" max="1" width="18.109375" style="72" customWidth="1"/>
+    <col min="2" max="2" width="43.6640625" style="72" customWidth="1"/>
+    <col min="3" max="1024" width="12.109375" style="72" customWidth="1"/>
+    <col min="1025" max="16384" width="43.6640625" style="74"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.4">
@@ -26425,14 +26422,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.88671875" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.33203125" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="7.0" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="20.109375" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="11.6640625" collapsed="false"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="15.5546875" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="16.0" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" width="9.5546875" collapsed="false"/>
+    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="9" max="9" width="9.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -26509,8 +26506,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="12.88671875" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="19.109375" collapsed="false"/>
+    <col min="1" max="1" width="12.88671875" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -26550,10 +26547,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.5546875" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="16.6640625" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="13.0" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="11.0" collapsed="false"/>
+    <col min="1" max="1" width="13.5546875" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -26599,28 +26596,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.88671875" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="18.109375" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="10.33203125" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="20.6640625" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="19.5546875" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="17.33203125" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="23.33203125" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="26.6640625" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" width="27.33203125" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="18.33203125" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" width="29.44140625" collapsed="false"/>
-    <col min="12" max="12" customWidth="true" width="16.6640625" collapsed="false"/>
-    <col min="13" max="13" customWidth="true" width="17.33203125" collapsed="false"/>
-    <col min="14" max="14" customWidth="true" width="16.33203125" collapsed="false"/>
-    <col min="15" max="15" customWidth="true" width="14.33203125" collapsed="false"/>
-    <col min="16" max="16" customWidth="true" width="15.5546875" collapsed="false"/>
-    <col min="17" max="17" customWidth="true" width="12.6640625" collapsed="false"/>
-    <col min="18" max="18" customWidth="true" width="13.33203125" collapsed="false"/>
-    <col min="19" max="19" customWidth="true" width="19.5546875" collapsed="false"/>
-    <col min="20" max="20" customWidth="true" width="13.33203125" collapsed="false"/>
-    <col min="21" max="21" customWidth="true" width="13.6640625" collapsed="false"/>
-    <col min="22" max="22" customWidth="true" style="108" width="14.44140625" collapsed="false"/>
+    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" customWidth="1"/>
+    <col min="8" max="8" width="26.6640625" customWidth="1"/>
+    <col min="9" max="9" width="27.33203125" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" customWidth="1"/>
+    <col min="11" max="11" width="29.44140625" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" customWidth="1"/>
+    <col min="13" max="13" width="17.33203125" customWidth="1"/>
+    <col min="14" max="14" width="16.33203125" customWidth="1"/>
+    <col min="15" max="15" width="14.33203125" customWidth="1"/>
+    <col min="16" max="16" width="15.5546875" customWidth="1"/>
+    <col min="17" max="17" width="12.6640625" customWidth="1"/>
+    <col min="18" max="18" width="13.33203125" customWidth="1"/>
+    <col min="19" max="19" width="19.5546875" customWidth="1"/>
+    <col min="20" max="20" width="13.33203125" customWidth="1"/>
+    <col min="21" max="21" width="13.6640625" customWidth="1"/>
+    <col min="22" max="22" width="14.44140625" style="108" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="94" customFormat="1">
@@ -26913,7 +26910,7 @@
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:AMJ7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:C1"/>
@@ -26921,10 +26918,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.33203125" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="81" width="16.0" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" style="81" width="22.6640625" collapsed="false"/>
-    <col min="3" max="1024" customWidth="true" style="81" width="16.0" collapsed="false"/>
-    <col min="1025" max="16384" style="82" width="10.33203125" collapsed="false"/>
+    <col min="1" max="1" width="16" style="81" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" style="81" customWidth="1"/>
+    <col min="3" max="1024" width="16" style="81" customWidth="1"/>
+    <col min="1025" max="16384" width="10.33203125" style="82"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -27021,31 +27018,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.33203125" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="19.109375" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="15.44140625" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="38.5546875" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="52.5546875" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="36.109375" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="34.33203125" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" width="30.109375" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="36.44140625" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" width="19.0" collapsed="false"/>
-    <col min="12" max="12" customWidth="true" width="37.33203125" collapsed="false"/>
-    <col min="13" max="13" customWidth="true" width="14.6640625" collapsed="false"/>
-    <col min="14" max="14" customWidth="true" width="15.33203125" collapsed="false"/>
-    <col min="15" max="15" customWidth="true" width="22.44140625" collapsed="false"/>
-    <col min="16" max="16" customWidth="true" width="30.6640625" collapsed="false"/>
-    <col min="17" max="17" customWidth="true" width="41.5546875" collapsed="false"/>
-    <col min="18" max="18" customWidth="true" width="25.109375" collapsed="false"/>
-    <col min="19" max="19" customWidth="true" width="29.88671875" collapsed="false"/>
-    <col min="20" max="20" customWidth="true" width="16.88671875" collapsed="false"/>
-    <col min="21" max="21" customWidth="true" width="15.109375" collapsed="false"/>
-    <col min="22" max="22" customWidth="true" width="18.5546875" collapsed="false"/>
-    <col min="23" max="23" customWidth="true" width="20.0" collapsed="false"/>
-    <col min="24" max="24" customWidth="true" width="17.109375" collapsed="false"/>
-    <col min="25" max="25" customWidth="true" width="21.0" collapsed="false"/>
-    <col min="26" max="26" customWidth="true" width="23.6640625" collapsed="false"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="5" max="5" width="38.5546875" customWidth="1"/>
+    <col min="6" max="6" width="52.5546875" customWidth="1"/>
+    <col min="7" max="7" width="36.109375" customWidth="1"/>
+    <col min="8" max="8" width="34.33203125" customWidth="1"/>
+    <col min="9" max="9" width="30.109375" customWidth="1"/>
+    <col min="10" max="10" width="36.44140625" customWidth="1"/>
+    <col min="11" max="11" width="19" customWidth="1"/>
+    <col min="12" max="12" width="37.33203125" customWidth="1"/>
+    <col min="13" max="13" width="14.6640625" customWidth="1"/>
+    <col min="14" max="14" width="15.33203125" customWidth="1"/>
+    <col min="15" max="15" width="22.44140625" customWidth="1"/>
+    <col min="16" max="16" width="30.6640625" customWidth="1"/>
+    <col min="17" max="17" width="41.5546875" customWidth="1"/>
+    <col min="18" max="18" width="25.109375" customWidth="1"/>
+    <col min="19" max="19" width="29.88671875" customWidth="1"/>
+    <col min="20" max="20" width="16.88671875" customWidth="1"/>
+    <col min="21" max="21" width="15.109375" customWidth="1"/>
+    <col min="22" max="22" width="18.5546875" customWidth="1"/>
+    <col min="23" max="23" width="20" customWidth="1"/>
+    <col min="24" max="24" width="17.109375" customWidth="1"/>
+    <col min="25" max="25" width="21" customWidth="1"/>
+    <col min="26" max="26" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
@@ -27226,14 +27223,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="32.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="42.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="30.6640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="42.109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="30.33203125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="29.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="39.33203125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="36.33203125" collapsed="true"/>
+    <col min="1" max="1" width="32.88671875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="42" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="42.109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="30.33203125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="29" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="39.33203125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="36.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -27828,15 +27825,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="32.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="42.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="42.0" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="30.6640625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="42.109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="30.33203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="29.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="39.33203125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="36.33203125" collapsed="true"/>
+    <col min="1" max="1" width="32.88671875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="42" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="42" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="42.109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30.33203125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="29" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="39.33203125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="36.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -27875,7 +27872,7 @@
       <c r="B2" s="25" t="s">
         <v>308</v>
       </c>
-      <c r="C2" s="134" t="s">
+      <c r="C2" s="123" t="s">
         <v>877</v>
       </c>
       <c r="D2" s="117" t="s">
@@ -27889,7 +27886,7 @@
       <c r="B3" s="25" t="s">
         <v>313</v>
       </c>
-      <c r="C3" s="135"/>
+      <c r="C3" s="124"/>
       <c r="D3" s="117" t="s">
         <v>127</v>
       </c>
@@ -27901,7 +27898,7 @@
       <c r="B4" s="25" t="s">
         <v>319</v>
       </c>
-      <c r="C4" s="135"/>
+      <c r="C4" s="124"/>
       <c r="D4" s="117" t="s">
         <v>127</v>
       </c>
@@ -27913,7 +27910,7 @@
       <c r="B5" s="25" t="s">
         <v>321</v>
       </c>
-      <c r="C5" s="135"/>
+      <c r="C5" s="124"/>
       <c r="D5" s="117" t="s">
         <v>127</v>
       </c>
@@ -27925,7 +27922,7 @@
       <c r="B6" s="25" t="s">
         <v>964</v>
       </c>
-      <c r="C6" s="135"/>
+      <c r="C6" s="124"/>
       <c r="D6" s="117" t="s">
         <v>127</v>
       </c>
@@ -27937,7 +27934,7 @@
       <c r="B7" s="25" t="s">
         <v>965</v>
       </c>
-      <c r="C7" s="135"/>
+      <c r="C7" s="124"/>
       <c r="D7" s="117" t="s">
         <v>127</v>
       </c>
@@ -27949,7 +27946,7 @@
       <c r="B8" s="25" t="s">
         <v>966</v>
       </c>
-      <c r="C8" s="135"/>
+      <c r="C8" s="124"/>
       <c r="D8" s="117" t="s">
         <v>127</v>
       </c>
@@ -27961,7 +27958,7 @@
       <c r="B9" s="25" t="s">
         <v>967</v>
       </c>
-      <c r="C9" s="135"/>
+      <c r="C9" s="124"/>
       <c r="D9" s="117" t="s">
         <v>127</v>
       </c>
@@ -27973,7 +27970,7 @@
       <c r="B10" s="25" t="s">
         <v>968</v>
       </c>
-      <c r="C10" s="135"/>
+      <c r="C10" s="124"/>
       <c r="D10" s="117" t="s">
         <v>127</v>
       </c>
@@ -27985,7 +27982,7 @@
       <c r="B11" s="25" t="s">
         <v>969</v>
       </c>
-      <c r="C11" s="136"/>
+      <c r="C11" s="125"/>
       <c r="D11" s="117" t="s">
         <v>127</v>
       </c>
@@ -27997,7 +27994,7 @@
       <c r="B12" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="C12" s="123" t="s">
+      <c r="C12" s="127" t="s">
         <v>949</v>
       </c>
       <c r="D12" s="117" t="s">
@@ -28011,7 +28008,7 @@
       <c r="B13" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="C13" s="123"/>
+      <c r="C13" s="127"/>
       <c r="D13" s="117" t="s">
         <v>127</v>
       </c>
@@ -28023,7 +28020,7 @@
       <c r="B14" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="C14" s="123"/>
+      <c r="C14" s="127"/>
       <c r="D14" s="117" t="s">
         <v>127</v>
       </c>
@@ -28035,7 +28032,7 @@
       <c r="B15" s="25" t="s">
         <v>178</v>
       </c>
-      <c r="C15" s="124" t="s">
+      <c r="C15" s="128" t="s">
         <v>950</v>
       </c>
       <c r="D15" s="117" t="s">
@@ -28049,7 +28046,7 @@
       <c r="B16" s="25" t="s">
         <v>213</v>
       </c>
-      <c r="C16" s="125"/>
+      <c r="C16" s="129"/>
       <c r="D16" s="117" t="s">
         <v>127</v>
       </c>
@@ -28061,7 +28058,7 @@
       <c r="B17" s="25" t="s">
         <v>217</v>
       </c>
-      <c r="C17" s="125"/>
+      <c r="C17" s="129"/>
       <c r="D17" s="117" t="s">
         <v>127</v>
       </c>
@@ -28073,7 +28070,7 @@
       <c r="B18" s="25" t="s">
         <v>218</v>
       </c>
-      <c r="C18" s="125"/>
+      <c r="C18" s="129"/>
       <c r="D18" s="117" t="s">
         <v>127</v>
       </c>
@@ -28085,7 +28082,7 @@
       <c r="B19" s="25" t="s">
         <v>220</v>
       </c>
-      <c r="C19" s="126"/>
+      <c r="C19" s="130"/>
       <c r="D19" s="117" t="s">
         <v>127</v>
       </c>
@@ -28100,7 +28097,7 @@
       <c r="B20" s="25" t="s">
         <v>230</v>
       </c>
-      <c r="C20" s="124" t="s">
+      <c r="C20" s="128" t="s">
         <v>951</v>
       </c>
       <c r="D20" s="117" t="s">
@@ -28114,7 +28111,7 @@
       <c r="B21" s="25" t="s">
         <v>232</v>
       </c>
-      <c r="C21" s="125"/>
+      <c r="C21" s="129"/>
       <c r="D21" s="117" t="s">
         <v>127</v>
       </c>
@@ -28126,7 +28123,7 @@
       <c r="B22" s="25" t="s">
         <v>234</v>
       </c>
-      <c r="C22" s="125"/>
+      <c r="C22" s="129"/>
       <c r="D22" s="117" t="s">
         <v>127</v>
       </c>
@@ -28138,7 +28135,7 @@
       <c r="B23" s="25" t="s">
         <v>237</v>
       </c>
-      <c r="C23" s="125"/>
+      <c r="C23" s="129"/>
       <c r="D23" s="117" t="s">
         <v>127</v>
       </c>
@@ -28150,7 +28147,7 @@
       <c r="B24" s="25" t="s">
         <v>243</v>
       </c>
-      <c r="C24" s="125"/>
+      <c r="C24" s="129"/>
       <c r="D24" s="117" t="s">
         <v>127</v>
       </c>
@@ -28162,7 +28159,7 @@
       <c r="B25" s="25" t="s">
         <v>239</v>
       </c>
-      <c r="C25" s="126"/>
+      <c r="C25" s="130"/>
       <c r="D25" s="117" t="s">
         <v>127</v>
       </c>
@@ -28174,7 +28171,7 @@
       <c r="B26" s="25" t="s">
         <v>246</v>
       </c>
-      <c r="C26" s="124" t="s">
+      <c r="C26" s="128" t="s">
         <v>952</v>
       </c>
       <c r="D26" s="117" t="s">
@@ -28188,7 +28185,7 @@
       <c r="B27" s="25" t="s">
         <v>248</v>
       </c>
-      <c r="C27" s="125"/>
+      <c r="C27" s="129"/>
       <c r="D27" s="117" t="s">
         <v>127</v>
       </c>
@@ -28200,7 +28197,7 @@
       <c r="B28" s="25" t="s">
         <v>250</v>
       </c>
-      <c r="C28" s="125"/>
+      <c r="C28" s="129"/>
       <c r="D28" s="117" t="s">
         <v>127</v>
       </c>
@@ -28212,7 +28209,7 @@
       <c r="B29" s="25" t="s">
         <v>252</v>
       </c>
-      <c r="C29" s="125"/>
+      <c r="C29" s="129"/>
       <c r="D29" s="117" t="s">
         <v>127</v>
       </c>
@@ -28224,7 +28221,7 @@
       <c r="B30" s="25" t="s">
         <v>255</v>
       </c>
-      <c r="C30" s="125"/>
+      <c r="C30" s="129"/>
       <c r="D30" s="117" t="s">
         <v>127</v>
       </c>
@@ -28236,7 +28233,7 @@
       <c r="B31" s="25" t="s">
         <v>257</v>
       </c>
-      <c r="C31" s="126"/>
+      <c r="C31" s="130"/>
       <c r="D31" s="117" t="s">
         <v>127</v>
       </c>
@@ -28248,7 +28245,7 @@
       <c r="B32" s="25" t="s">
         <v>273</v>
       </c>
-      <c r="C32" s="124" t="s">
+      <c r="C32" s="128" t="s">
         <v>953</v>
       </c>
       <c r="D32" s="117" t="s">
@@ -28262,7 +28259,7 @@
       <c r="B33" s="25" t="s">
         <v>271</v>
       </c>
-      <c r="C33" s="125"/>
+      <c r="C33" s="129"/>
       <c r="D33" s="117" t="s">
         <v>127</v>
       </c>
@@ -28274,7 +28271,7 @@
       <c r="B34" s="25" t="s">
         <v>285</v>
       </c>
-      <c r="C34" s="125"/>
+      <c r="C34" s="129"/>
       <c r="D34" s="117" t="s">
         <v>127</v>
       </c>
@@ -28286,7 +28283,7 @@
       <c r="B35" s="25" t="s">
         <v>288</v>
       </c>
-      <c r="C35" s="125"/>
+      <c r="C35" s="129"/>
       <c r="D35" s="117" t="s">
         <v>127</v>
       </c>
@@ -28298,7 +28295,7 @@
       <c r="B36" s="25" t="s">
         <v>290</v>
       </c>
-      <c r="C36" s="126"/>
+      <c r="C36" s="130"/>
       <c r="D36" s="117" t="s">
         <v>127</v>
       </c>
@@ -28310,7 +28307,7 @@
       <c r="B37" s="25" t="s">
         <v>367</v>
       </c>
-      <c r="C37" s="127" t="s">
+      <c r="C37" s="131" t="s">
         <v>954</v>
       </c>
       <c r="D37" s="117" t="s">
@@ -28324,7 +28321,7 @@
       <c r="B38" s="25" t="s">
         <v>379</v>
       </c>
-      <c r="C38" s="128"/>
+      <c r="C38" s="132"/>
       <c r="D38" s="117" t="s">
         <v>127</v>
       </c>
@@ -28336,7 +28333,7 @@
       <c r="B39" s="25" t="s">
         <v>384</v>
       </c>
-      <c r="C39" s="128"/>
+      <c r="C39" s="132"/>
       <c r="D39" s="117" t="s">
         <v>127</v>
       </c>
@@ -28348,7 +28345,7 @@
       <c r="B40" s="25" t="s">
         <v>389</v>
       </c>
-      <c r="C40" s="128"/>
+      <c r="C40" s="132"/>
       <c r="D40" s="117" t="s">
         <v>127</v>
       </c>
@@ -28360,7 +28357,7 @@
       <c r="B41" s="25" t="s">
         <v>391</v>
       </c>
-      <c r="C41" s="128"/>
+      <c r="C41" s="132"/>
       <c r="D41" s="117" t="s">
         <v>127</v>
       </c>
@@ -28372,7 +28369,7 @@
       <c r="B42" s="25" t="s">
         <v>394</v>
       </c>
-      <c r="C42" s="128"/>
+      <c r="C42" s="132"/>
       <c r="D42" s="117" t="s">
         <v>127</v>
       </c>
@@ -28384,7 +28381,7 @@
       <c r="B43" s="25" t="s">
         <v>398</v>
       </c>
-      <c r="C43" s="128"/>
+      <c r="C43" s="132"/>
       <c r="D43" s="117" t="s">
         <v>127</v>
       </c>
@@ -28396,7 +28393,7 @@
       <c r="B44" s="25" t="s">
         <v>402</v>
       </c>
-      <c r="C44" s="128"/>
+      <c r="C44" s="132"/>
       <c r="D44" s="117" t="s">
         <v>127</v>
       </c>
@@ -28408,7 +28405,7 @@
       <c r="B45" s="25" t="s">
         <v>404</v>
       </c>
-      <c r="C45" s="128"/>
+      <c r="C45" s="132"/>
       <c r="D45" s="117" t="s">
         <v>127</v>
       </c>
@@ -28420,7 +28417,7 @@
       <c r="B46" s="25" t="s">
         <v>406</v>
       </c>
-      <c r="C46" s="128"/>
+      <c r="C46" s="132"/>
       <c r="D46" s="117" t="s">
         <v>127</v>
       </c>
@@ -28432,7 +28429,7 @@
       <c r="B47" s="25" t="s">
         <v>408</v>
       </c>
-      <c r="C47" s="128"/>
+      <c r="C47" s="132"/>
       <c r="D47" s="117" t="s">
         <v>127</v>
       </c>
@@ -28444,7 +28441,7 @@
       <c r="B48" s="25" t="s">
         <v>410</v>
       </c>
-      <c r="C48" s="129"/>
+      <c r="C48" s="133"/>
       <c r="D48" s="117" t="s">
         <v>127</v>
       </c>
@@ -28456,7 +28453,7 @@
       <c r="B49" s="25" t="s">
         <v>615</v>
       </c>
-      <c r="C49" s="127" t="s">
+      <c r="C49" s="131" t="s">
         <v>955</v>
       </c>
       <c r="D49" s="117" t="s">
@@ -28470,7 +28467,7 @@
       <c r="B50" s="25" t="s">
         <v>617</v>
       </c>
-      <c r="C50" s="128"/>
+      <c r="C50" s="132"/>
       <c r="D50" s="117" t="s">
         <v>127</v>
       </c>
@@ -28482,7 +28479,7 @@
       <c r="B51" s="25" t="s">
         <v>620</v>
       </c>
-      <c r="C51" s="129"/>
+      <c r="C51" s="133"/>
       <c r="D51" s="117" t="s">
         <v>127</v>
       </c>
@@ -28494,7 +28491,7 @@
       <c r="B52" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="C52" s="124" t="s">
+      <c r="C52" s="128" t="s">
         <v>956</v>
       </c>
       <c r="D52" s="117" t="s">
@@ -28508,7 +28505,7 @@
       <c r="B53" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="C53" s="125"/>
+      <c r="C53" s="129"/>
       <c r="D53" s="117" t="s">
         <v>127</v>
       </c>
@@ -28520,7 +28517,7 @@
       <c r="B54" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="C54" s="125"/>
+      <c r="C54" s="129"/>
       <c r="D54" s="117" t="s">
         <v>127</v>
       </c>
@@ -28532,7 +28529,7 @@
       <c r="B55" s="25" t="s">
         <v>876</v>
       </c>
-      <c r="C55" s="125"/>
+      <c r="C55" s="129"/>
       <c r="D55" s="117" t="s">
         <v>127</v>
       </c>
@@ -28544,7 +28541,7 @@
       <c r="B56" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="C56" s="125"/>
+      <c r="C56" s="129"/>
       <c r="D56" s="117" t="s">
         <v>127</v>
       </c>
@@ -28556,7 +28553,7 @@
       <c r="B57" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="C57" s="126"/>
+      <c r="C57" s="130"/>
       <c r="D57" s="117" t="s">
         <v>127</v>
       </c>
@@ -28568,7 +28565,7 @@
       <c r="B58" s="25" t="s">
         <v>428</v>
       </c>
-      <c r="C58" s="130" t="s">
+      <c r="C58" s="134" t="s">
         <v>957</v>
       </c>
       <c r="D58" s="117" t="s">
@@ -28582,7 +28579,7 @@
       <c r="B59" s="25" t="s">
         <v>430</v>
       </c>
-      <c r="C59" s="131"/>
+      <c r="C59" s="135"/>
       <c r="D59" s="117" t="s">
         <v>127</v>
       </c>
@@ -28594,7 +28591,7 @@
       <c r="B60" s="25" t="s">
         <v>438</v>
       </c>
-      <c r="C60" s="131"/>
+      <c r="C60" s="135"/>
       <c r="D60" s="117" t="s">
         <v>127</v>
       </c>
@@ -28606,7 +28603,7 @@
       <c r="B61" s="25" t="s">
         <v>446</v>
       </c>
-      <c r="C61" s="131"/>
+      <c r="C61" s="135"/>
       <c r="D61" s="117" t="s">
         <v>127</v>
       </c>
@@ -28618,7 +28615,7 @@
       <c r="B62" s="25" t="s">
         <v>449</v>
       </c>
-      <c r="C62" s="131"/>
+      <c r="C62" s="135"/>
       <c r="D62" s="117" t="s">
         <v>127</v>
       </c>
@@ -28630,7 +28627,7 @@
       <c r="B63" s="25" t="s">
         <v>452</v>
       </c>
-      <c r="C63" s="131"/>
+      <c r="C63" s="135"/>
       <c r="D63" s="117" t="s">
         <v>127</v>
       </c>
@@ -28642,7 +28639,7 @@
       <c r="B64" s="25" t="s">
         <v>454</v>
       </c>
-      <c r="C64" s="131"/>
+      <c r="C64" s="135"/>
       <c r="D64" s="117" t="s">
         <v>127</v>
       </c>
@@ -28654,7 +28651,7 @@
       <c r="B65" s="25" t="s">
         <v>458</v>
       </c>
-      <c r="C65" s="132"/>
+      <c r="C65" s="136"/>
       <c r="D65" s="117" t="s">
         <v>127</v>
       </c>
@@ -28666,7 +28663,7 @@
       <c r="B66" s="25" t="s">
         <v>892</v>
       </c>
-      <c r="C66" s="133" t="s">
+      <c r="C66" s="126" t="s">
         <v>881</v>
       </c>
       <c r="D66" s="117" t="s">
@@ -28680,7 +28677,7 @@
       <c r="B67" s="25" t="s">
         <v>893</v>
       </c>
-      <c r="C67" s="133"/>
+      <c r="C67" s="126"/>
       <c r="D67" s="117" t="s">
         <v>127</v>
       </c>
@@ -28806,7 +28803,7 @@
       <c r="B77" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="C77" s="133" t="s">
+      <c r="C77" s="126" t="s">
         <v>883</v>
       </c>
       <c r="D77" s="117" t="s">
@@ -28820,7 +28817,7 @@
       <c r="B78" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="C78" s="133"/>
+      <c r="C78" s="126"/>
       <c r="D78" s="117" t="s">
         <v>127</v>
       </c>
@@ -28846,7 +28843,7 @@
       <c r="B80" s="25" t="s">
         <v>532</v>
       </c>
-      <c r="C80" s="133" t="s">
+      <c r="C80" s="126" t="s">
         <v>885</v>
       </c>
       <c r="D80" s="117" t="s">
@@ -28860,7 +28857,7 @@
       <c r="B81" s="25" t="s">
         <v>534</v>
       </c>
-      <c r="C81" s="133"/>
+      <c r="C81" s="126"/>
       <c r="D81" s="117" t="s">
         <v>127</v>
       </c>
@@ -28872,7 +28869,7 @@
       <c r="B82" s="25" t="s">
         <v>537</v>
       </c>
-      <c r="C82" s="133"/>
+      <c r="C82" s="126"/>
       <c r="D82" s="117" t="s">
         <v>127</v>
       </c>
@@ -28884,7 +28881,7 @@
       <c r="B83" s="25" t="s">
         <v>737</v>
       </c>
-      <c r="C83" s="133" t="s">
+      <c r="C83" s="126" t="s">
         <v>886</v>
       </c>
       <c r="D83" s="117" t="s">
@@ -28898,7 +28895,7 @@
       <c r="B84" s="25" t="s">
         <v>744</v>
       </c>
-      <c r="C84" s="133"/>
+      <c r="C84" s="126"/>
       <c r="D84" s="117" t="s">
         <v>127</v>
       </c>
@@ -28910,7 +28907,7 @@
       <c r="B85" s="25" t="s">
         <v>746</v>
       </c>
-      <c r="C85" s="133"/>
+      <c r="C85" s="126"/>
       <c r="D85" s="117" t="s">
         <v>127</v>
       </c>
@@ -28922,7 +28919,7 @@
       <c r="B86" s="25" t="s">
         <v>748</v>
       </c>
-      <c r="C86" s="133"/>
+      <c r="C86" s="126"/>
       <c r="D86" s="117" t="s">
         <v>127</v>
       </c>
@@ -28934,7 +28931,7 @@
       <c r="B87" s="25" t="s">
         <v>750</v>
       </c>
-      <c r="C87" s="133"/>
+      <c r="C87" s="126"/>
       <c r="D87" s="117" t="s">
         <v>127</v>
       </c>
@@ -28946,7 +28943,7 @@
       <c r="B88" s="25" t="s">
         <v>720</v>
       </c>
-      <c r="C88" s="133" t="s">
+      <c r="C88" s="126" t="s">
         <v>887</v>
       </c>
       <c r="D88" s="117" t="s">
@@ -28960,7 +28957,7 @@
       <c r="B89" s="25" t="s">
         <v>722</v>
       </c>
-      <c r="C89" s="133"/>
+      <c r="C89" s="126"/>
       <c r="D89" s="117" t="s">
         <v>127</v>
       </c>
@@ -29785,6 +29782,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="C90:C93"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="C15:C19"/>
+    <mergeCell ref="C20:C25"/>
+    <mergeCell ref="C26:C31"/>
+    <mergeCell ref="C32:C36"/>
+    <mergeCell ref="C37:C48"/>
+    <mergeCell ref="C49:C51"/>
+    <mergeCell ref="C52:C57"/>
+    <mergeCell ref="C58:C65"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="C68:C70"/>
+    <mergeCell ref="C71:C75"/>
     <mergeCell ref="C153:C155"/>
     <mergeCell ref="C2:C11"/>
     <mergeCell ref="C119:C122"/>
@@ -29801,19 +29811,6 @@
     <mergeCell ref="C80:C82"/>
     <mergeCell ref="C83:C87"/>
     <mergeCell ref="C88:C89"/>
-    <mergeCell ref="C90:C93"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="C15:C19"/>
-    <mergeCell ref="C20:C25"/>
-    <mergeCell ref="C26:C31"/>
-    <mergeCell ref="C32:C36"/>
-    <mergeCell ref="C37:C48"/>
-    <mergeCell ref="C49:C51"/>
-    <mergeCell ref="C52:C57"/>
-    <mergeCell ref="C58:C65"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="C68:C70"/>
-    <mergeCell ref="C71:C75"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:B1048576 C1:C2 C12:C1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="4"/>
@@ -29840,35 +29837,35 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="24.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="37.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="26.44140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="3" width="18.88671875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="21.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="3" width="19.88671875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="3" width="21.88671875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="3" width="30.6640625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="3" width="31.6640625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="3" width="29.109375" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="3" width="28.33203125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="3" width="25.0" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="3" width="21.109375" collapsed="true"/>
-    <col min="14" max="15" style="3" width="9.109375" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" style="3" width="17.44140625" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" style="3" width="26.88671875" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" style="3" width="16.5546875" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" style="3" width="20.0" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" style="3" width="13.5546875" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" style="3" width="22.109375" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" style="3" width="21.33203125" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" style="3" width="43.33203125" collapsed="true"/>
-    <col min="24" max="24" style="3" width="9.109375" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" style="3" width="18.109375" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" style="3" width="20.0" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" style="3" width="23.44140625" collapsed="true"/>
-    <col min="28" max="28" customWidth="true" style="3" width="27.0" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" style="3" width="23.88671875" collapsed="true"/>
-    <col min="30" max="16384" style="3" width="9.109375" collapsed="true"/>
+    <col min="1" max="1" width="24.109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="37.6640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.44140625" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.88671875" style="3" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21" style="3" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.88671875" style="3" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.88671875" style="3" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="30.6640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="31.6640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="29.109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="28.33203125" style="3" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="25" style="3" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="21.109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="14" max="15" width="9.109375" style="3" collapsed="1"/>
+    <col min="16" max="16" width="17.44140625" style="3" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="26.88671875" style="3" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="16.5546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="20" style="3" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="13.5546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="22.109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="21.33203125" style="3" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="43.33203125" style="3" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9.109375" style="3" collapsed="1"/>
+    <col min="25" max="25" width="18.109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="20" style="3" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="23.44140625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="27" style="3" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="23.88671875" style="3" customWidth="1" collapsed="1"/>
+    <col min="30" max="16384" width="9.109375" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
@@ -30232,18 +30229,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="23.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="30.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="26.88671875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="3" width="24.6640625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="29.88671875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="3" width="25.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="3" width="36.88671875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="3" width="15.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="3" width="22.6640625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="3" width="17.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="3" width="19.109375" collapsed="true"/>
-    <col min="12" max="16384" style="3" width="9.109375" collapsed="true"/>
+    <col min="1" max="1" width="23" style="3" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30" style="3" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.88671875" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.6640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="29.88671875" style="3" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="25" style="3" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="36.88671875" style="3" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15" style="3" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="22.6640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17" style="3" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="19.109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="9.109375" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -30436,31 +30433,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="24.88671875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="12.88671875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.33203125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="30.5546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="17.109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="26.6640625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="17.44140625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="15.88671875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="14.33203125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="14.88671875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="18.44140625" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="16.109375" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="11.44140625" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="16.109375" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="19.44140625" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" width="24.6640625" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" width="14.109375" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" width="13.5546875" collapsed="true"/>
-    <col min="28" max="28" customWidth="true" width="17.109375" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.88671875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="26.6640625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.44140625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15.88671875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="14.33203125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.88671875" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="18.44140625" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="13.33203125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="16.109375" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="11.44140625" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="16.109375" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="19.44140625" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="24.6640625" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="14.109375" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="18.6640625" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="25" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="13.5546875" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="17.109375" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="18" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
@@ -30857,21 +30854,21 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="21.5546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="30.33203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="27.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="3" width="25.5546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="28.33203125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="3" width="31.88671875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="3" width="33.5546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="3" width="29.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="3" width="24.44140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="3" width="20.6640625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="3" width="26.6640625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="3" width="15.109375" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="3" width="28.33203125" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" style="3" width="22.88671875" collapsed="true"/>
-    <col min="15" max="16384" style="3" width="9.109375" collapsed="true"/>
+    <col min="1" max="1" width="21.5546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.33203125" style="3" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="27" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.5546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="28.33203125" style="3" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="31.88671875" style="3" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="33.5546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="29" style="3" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="24.44140625" style="3" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.6640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="26.6640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="28.33203125" style="3" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="22.88671875" style="3" customWidth="1" collapsed="1"/>
+    <col min="15" max="16384" width="9.109375" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -31090,29 +31087,29 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.88671875" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="26.6640625" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="13.44140625" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="29.44140625" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="57.33203125" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="32.109375" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="28.88671875" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" width="26.88671875" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="29.33203125" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" width="17.6640625" collapsed="false"/>
-    <col min="12" max="12" customWidth="true" width="34.33203125" collapsed="false"/>
-    <col min="13" max="13" customWidth="true" width="14.6640625" collapsed="false"/>
-    <col min="14" max="14" customWidth="true" width="13.0" collapsed="false"/>
-    <col min="15" max="15" customWidth="true" width="16.44140625" collapsed="false"/>
-    <col min="16" max="16" customWidth="true" width="26.0" collapsed="false"/>
-    <col min="17" max="17" customWidth="true" width="32.88671875" collapsed="false"/>
-    <col min="18" max="18" customWidth="true" width="13.88671875" collapsed="false"/>
-    <col min="19" max="19" customWidth="true" width="16.44140625" collapsed="false"/>
-    <col min="20" max="20" customWidth="true" width="15.44140625" collapsed="false"/>
-    <col min="21" max="21" customWidth="true" width="27.109375" collapsed="false"/>
-    <col min="22" max="22" customWidth="true" width="14.0" collapsed="false"/>
-    <col min="23" max="23" customWidth="true" width="17.44140625" collapsed="false"/>
-    <col min="24" max="24" customWidth="true" width="17.0" collapsed="false"/>
+    <col min="1" max="1" width="20.88671875" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" customWidth="1"/>
+    <col min="5" max="5" width="29.44140625" customWidth="1"/>
+    <col min="6" max="6" width="57.33203125" customWidth="1"/>
+    <col min="7" max="7" width="32.109375" customWidth="1"/>
+    <col min="8" max="8" width="28.88671875" customWidth="1"/>
+    <col min="9" max="9" width="26.88671875" customWidth="1"/>
+    <col min="10" max="10" width="29.33203125" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" customWidth="1"/>
+    <col min="12" max="12" width="34.33203125" customWidth="1"/>
+    <col min="13" max="13" width="14.6640625" customWidth="1"/>
+    <col min="14" max="14" width="13" customWidth="1"/>
+    <col min="15" max="15" width="16.44140625" customWidth="1"/>
+    <col min="16" max="16" width="26" customWidth="1"/>
+    <col min="17" max="17" width="32.88671875" customWidth="1"/>
+    <col min="18" max="18" width="13.88671875" customWidth="1"/>
+    <col min="19" max="19" width="16.44140625" customWidth="1"/>
+    <col min="20" max="20" width="15.44140625" customWidth="1"/>
+    <col min="21" max="21" width="27.109375" customWidth="1"/>
+    <col min="22" max="22" width="14" customWidth="1"/>
+    <col min="23" max="23" width="17.44140625" customWidth="1"/>
+    <col min="24" max="24" width="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -32003,24 +32000,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.6640625" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="15.0" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="14.109375" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="11.33203125" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="14.88671875" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="14.33203125" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="15.0" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="15.6640625" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" width="16.88671875" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="13.44140625" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" width="16.109375" collapsed="false"/>
-    <col min="12" max="12" customWidth="true" width="16.6640625" collapsed="false"/>
-    <col min="15" max="15" customWidth="true" width="14.0" collapsed="false"/>
-    <col min="16" max="16" customWidth="true" width="15.5546875" collapsed="false"/>
-    <col min="17" max="17" customWidth="true" width="11.0" collapsed="false"/>
-    <col min="18" max="18" customWidth="true" width="17.44140625" collapsed="false"/>
-    <col min="20" max="20" customWidth="true" width="10.5546875" collapsed="false"/>
-    <col min="21" max="21" customWidth="true" width="14.44140625" collapsed="false"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
+    <col min="9" max="9" width="16.88671875" customWidth="1"/>
+    <col min="10" max="10" width="13.44140625" customWidth="1"/>
+    <col min="11" max="11" width="16.109375" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" customWidth="1"/>
+    <col min="15" max="15" width="14" customWidth="1"/>
+    <col min="16" max="16" width="15.5546875" customWidth="1"/>
+    <col min="17" max="17" width="11" customWidth="1"/>
+    <col min="18" max="18" width="17.44140625" customWidth="1"/>
+    <col min="20" max="20" width="10.5546875" customWidth="1"/>
+    <col min="21" max="21" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">

</xml_diff>

<commit_message>
Ijarah - CF debt, Application details, Income details, Underwriter & offer Details testcases are updated.........
</commit_message>
<xml_diff>
--- a/ULS_Ijarah_MainRepository/TestData/IjarahTestData.xlsx
+++ b/ULS_Ijarah_MainRepository/TestData/IjarahTestData.xlsx
@@ -2987,13 +2987,13 @@
     <t>UserReturn</t>
   </si>
   <si>
-    <t>01069</t>
-  </si>
-  <si>
     <t>0362</t>
   </si>
   <si>
     <t>0365</t>
+  </si>
+  <si>
+    <t>0371</t>
   </si>
 </sst>
 </file>
@@ -3758,18 +3758,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3798,6 +3786,18 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4156,7 +4156,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -4184,7 +4184,7 @@
         <v>977</v>
       </c>
       <c r="B2" s="120" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="C2" s="121" t="s">
         <v>6</v>
@@ -4284,7 +4284,7 @@
         <v>625</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>6</v>
@@ -4350,7 +4350,7 @@
         <v>850</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="C17" s="83" t="s">
         <v>6</v>
@@ -27872,7 +27872,7 @@
       <c r="B2" s="25" t="s">
         <v>308</v>
       </c>
-      <c r="C2" s="123" t="s">
+      <c r="C2" s="134" t="s">
         <v>877</v>
       </c>
       <c r="D2" s="117" t="s">
@@ -27886,7 +27886,7 @@
       <c r="B3" s="25" t="s">
         <v>313</v>
       </c>
-      <c r="C3" s="124"/>
+      <c r="C3" s="135"/>
       <c r="D3" s="117" t="s">
         <v>127</v>
       </c>
@@ -27898,7 +27898,7 @@
       <c r="B4" s="25" t="s">
         <v>319</v>
       </c>
-      <c r="C4" s="124"/>
+      <c r="C4" s="135"/>
       <c r="D4" s="117" t="s">
         <v>127</v>
       </c>
@@ -27910,7 +27910,7 @@
       <c r="B5" s="25" t="s">
         <v>321</v>
       </c>
-      <c r="C5" s="124"/>
+      <c r="C5" s="135"/>
       <c r="D5" s="117" t="s">
         <v>127</v>
       </c>
@@ -27922,7 +27922,7 @@
       <c r="B6" s="25" t="s">
         <v>964</v>
       </c>
-      <c r="C6" s="124"/>
+      <c r="C6" s="135"/>
       <c r="D6" s="117" t="s">
         <v>127</v>
       </c>
@@ -27934,7 +27934,7 @@
       <c r="B7" s="25" t="s">
         <v>965</v>
       </c>
-      <c r="C7" s="124"/>
+      <c r="C7" s="135"/>
       <c r="D7" s="117" t="s">
         <v>127</v>
       </c>
@@ -27946,7 +27946,7 @@
       <c r="B8" s="25" t="s">
         <v>966</v>
       </c>
-      <c r="C8" s="124"/>
+      <c r="C8" s="135"/>
       <c r="D8" s="117" t="s">
         <v>127</v>
       </c>
@@ -27958,7 +27958,7 @@
       <c r="B9" s="25" t="s">
         <v>967</v>
       </c>
-      <c r="C9" s="124"/>
+      <c r="C9" s="135"/>
       <c r="D9" s="117" t="s">
         <v>127</v>
       </c>
@@ -27970,7 +27970,7 @@
       <c r="B10" s="25" t="s">
         <v>968</v>
       </c>
-      <c r="C10" s="124"/>
+      <c r="C10" s="135"/>
       <c r="D10" s="117" t="s">
         <v>127</v>
       </c>
@@ -27982,7 +27982,7 @@
       <c r="B11" s="25" t="s">
         <v>969</v>
       </c>
-      <c r="C11" s="125"/>
+      <c r="C11" s="136"/>
       <c r="D11" s="117" t="s">
         <v>127</v>
       </c>
@@ -27994,7 +27994,7 @@
       <c r="B12" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="C12" s="127" t="s">
+      <c r="C12" s="123" t="s">
         <v>949</v>
       </c>
       <c r="D12" s="117" t="s">
@@ -28008,7 +28008,7 @@
       <c r="B13" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="C13" s="127"/>
+      <c r="C13" s="123"/>
       <c r="D13" s="117" t="s">
         <v>127</v>
       </c>
@@ -28020,7 +28020,7 @@
       <c r="B14" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="C14" s="127"/>
+      <c r="C14" s="123"/>
       <c r="D14" s="117" t="s">
         <v>127</v>
       </c>
@@ -28032,7 +28032,7 @@
       <c r="B15" s="25" t="s">
         <v>178</v>
       </c>
-      <c r="C15" s="128" t="s">
+      <c r="C15" s="124" t="s">
         <v>950</v>
       </c>
       <c r="D15" s="117" t="s">
@@ -28046,7 +28046,7 @@
       <c r="B16" s="25" t="s">
         <v>213</v>
       </c>
-      <c r="C16" s="129"/>
+      <c r="C16" s="125"/>
       <c r="D16" s="117" t="s">
         <v>127</v>
       </c>
@@ -28058,7 +28058,7 @@
       <c r="B17" s="25" t="s">
         <v>217</v>
       </c>
-      <c r="C17" s="129"/>
+      <c r="C17" s="125"/>
       <c r="D17" s="117" t="s">
         <v>127</v>
       </c>
@@ -28070,7 +28070,7 @@
       <c r="B18" s="25" t="s">
         <v>218</v>
       </c>
-      <c r="C18" s="129"/>
+      <c r="C18" s="125"/>
       <c r="D18" s="117" t="s">
         <v>127</v>
       </c>
@@ -28082,7 +28082,7 @@
       <c r="B19" s="25" t="s">
         <v>220</v>
       </c>
-      <c r="C19" s="130"/>
+      <c r="C19" s="126"/>
       <c r="D19" s="117" t="s">
         <v>127</v>
       </c>
@@ -28097,7 +28097,7 @@
       <c r="B20" s="25" t="s">
         <v>230</v>
       </c>
-      <c r="C20" s="128" t="s">
+      <c r="C20" s="124" t="s">
         <v>951</v>
       </c>
       <c r="D20" s="117" t="s">
@@ -28111,7 +28111,7 @@
       <c r="B21" s="25" t="s">
         <v>232</v>
       </c>
-      <c r="C21" s="129"/>
+      <c r="C21" s="125"/>
       <c r="D21" s="117" t="s">
         <v>127</v>
       </c>
@@ -28123,7 +28123,7 @@
       <c r="B22" s="25" t="s">
         <v>234</v>
       </c>
-      <c r="C22" s="129"/>
+      <c r="C22" s="125"/>
       <c r="D22" s="117" t="s">
         <v>127</v>
       </c>
@@ -28135,7 +28135,7 @@
       <c r="B23" s="25" t="s">
         <v>237</v>
       </c>
-      <c r="C23" s="129"/>
+      <c r="C23" s="125"/>
       <c r="D23" s="117" t="s">
         <v>127</v>
       </c>
@@ -28147,7 +28147,7 @@
       <c r="B24" s="25" t="s">
         <v>243</v>
       </c>
-      <c r="C24" s="129"/>
+      <c r="C24" s="125"/>
       <c r="D24" s="117" t="s">
         <v>127</v>
       </c>
@@ -28159,7 +28159,7 @@
       <c r="B25" s="25" t="s">
         <v>239</v>
       </c>
-      <c r="C25" s="130"/>
+      <c r="C25" s="126"/>
       <c r="D25" s="117" t="s">
         <v>127</v>
       </c>
@@ -28171,7 +28171,7 @@
       <c r="B26" s="25" t="s">
         <v>246</v>
       </c>
-      <c r="C26" s="128" t="s">
+      <c r="C26" s="124" t="s">
         <v>952</v>
       </c>
       <c r="D26" s="117" t="s">
@@ -28185,7 +28185,7 @@
       <c r="B27" s="25" t="s">
         <v>248</v>
       </c>
-      <c r="C27" s="129"/>
+      <c r="C27" s="125"/>
       <c r="D27" s="117" t="s">
         <v>127</v>
       </c>
@@ -28197,7 +28197,7 @@
       <c r="B28" s="25" t="s">
         <v>250</v>
       </c>
-      <c r="C28" s="129"/>
+      <c r="C28" s="125"/>
       <c r="D28" s="117" t="s">
         <v>127</v>
       </c>
@@ -28209,7 +28209,7 @@
       <c r="B29" s="25" t="s">
         <v>252</v>
       </c>
-      <c r="C29" s="129"/>
+      <c r="C29" s="125"/>
       <c r="D29" s="117" t="s">
         <v>127</v>
       </c>
@@ -28221,7 +28221,7 @@
       <c r="B30" s="25" t="s">
         <v>255</v>
       </c>
-      <c r="C30" s="129"/>
+      <c r="C30" s="125"/>
       <c r="D30" s="117" t="s">
         <v>127</v>
       </c>
@@ -28233,7 +28233,7 @@
       <c r="B31" s="25" t="s">
         <v>257</v>
       </c>
-      <c r="C31" s="130"/>
+      <c r="C31" s="126"/>
       <c r="D31" s="117" t="s">
         <v>127</v>
       </c>
@@ -28245,7 +28245,7 @@
       <c r="B32" s="25" t="s">
         <v>273</v>
       </c>
-      <c r="C32" s="128" t="s">
+      <c r="C32" s="124" t="s">
         <v>953</v>
       </c>
       <c r="D32" s="117" t="s">
@@ -28259,7 +28259,7 @@
       <c r="B33" s="25" t="s">
         <v>271</v>
       </c>
-      <c r="C33" s="129"/>
+      <c r="C33" s="125"/>
       <c r="D33" s="117" t="s">
         <v>127</v>
       </c>
@@ -28271,7 +28271,7 @@
       <c r="B34" s="25" t="s">
         <v>285</v>
       </c>
-      <c r="C34" s="129"/>
+      <c r="C34" s="125"/>
       <c r="D34" s="117" t="s">
         <v>127</v>
       </c>
@@ -28283,7 +28283,7 @@
       <c r="B35" s="25" t="s">
         <v>288</v>
       </c>
-      <c r="C35" s="129"/>
+      <c r="C35" s="125"/>
       <c r="D35" s="117" t="s">
         <v>127</v>
       </c>
@@ -28295,7 +28295,7 @@
       <c r="B36" s="25" t="s">
         <v>290</v>
       </c>
-      <c r="C36" s="130"/>
+      <c r="C36" s="126"/>
       <c r="D36" s="117" t="s">
         <v>127</v>
       </c>
@@ -28307,7 +28307,7 @@
       <c r="B37" s="25" t="s">
         <v>367</v>
       </c>
-      <c r="C37" s="131" t="s">
+      <c r="C37" s="127" t="s">
         <v>954</v>
       </c>
       <c r="D37" s="117" t="s">
@@ -28321,7 +28321,7 @@
       <c r="B38" s="25" t="s">
         <v>379</v>
       </c>
-      <c r="C38" s="132"/>
+      <c r="C38" s="128"/>
       <c r="D38" s="117" t="s">
         <v>127</v>
       </c>
@@ -28333,7 +28333,7 @@
       <c r="B39" s="25" t="s">
         <v>384</v>
       </c>
-      <c r="C39" s="132"/>
+      <c r="C39" s="128"/>
       <c r="D39" s="117" t="s">
         <v>127</v>
       </c>
@@ -28345,7 +28345,7 @@
       <c r="B40" s="25" t="s">
         <v>389</v>
       </c>
-      <c r="C40" s="132"/>
+      <c r="C40" s="128"/>
       <c r="D40" s="117" t="s">
         <v>127</v>
       </c>
@@ -28357,7 +28357,7 @@
       <c r="B41" s="25" t="s">
         <v>391</v>
       </c>
-      <c r="C41" s="132"/>
+      <c r="C41" s="128"/>
       <c r="D41" s="117" t="s">
         <v>127</v>
       </c>
@@ -28369,7 +28369,7 @@
       <c r="B42" s="25" t="s">
         <v>394</v>
       </c>
-      <c r="C42" s="132"/>
+      <c r="C42" s="128"/>
       <c r="D42" s="117" t="s">
         <v>127</v>
       </c>
@@ -28381,7 +28381,7 @@
       <c r="B43" s="25" t="s">
         <v>398</v>
       </c>
-      <c r="C43" s="132"/>
+      <c r="C43" s="128"/>
       <c r="D43" s="117" t="s">
         <v>127</v>
       </c>
@@ -28393,7 +28393,7 @@
       <c r="B44" s="25" t="s">
         <v>402</v>
       </c>
-      <c r="C44" s="132"/>
+      <c r="C44" s="128"/>
       <c r="D44" s="117" t="s">
         <v>127</v>
       </c>
@@ -28405,7 +28405,7 @@
       <c r="B45" s="25" t="s">
         <v>404</v>
       </c>
-      <c r="C45" s="132"/>
+      <c r="C45" s="128"/>
       <c r="D45" s="117" t="s">
         <v>127</v>
       </c>
@@ -28417,7 +28417,7 @@
       <c r="B46" s="25" t="s">
         <v>406</v>
       </c>
-      <c r="C46" s="132"/>
+      <c r="C46" s="128"/>
       <c r="D46" s="117" t="s">
         <v>127</v>
       </c>
@@ -28429,7 +28429,7 @@
       <c r="B47" s="25" t="s">
         <v>408</v>
       </c>
-      <c r="C47" s="132"/>
+      <c r="C47" s="128"/>
       <c r="D47" s="117" t="s">
         <v>127</v>
       </c>
@@ -28441,7 +28441,7 @@
       <c r="B48" s="25" t="s">
         <v>410</v>
       </c>
-      <c r="C48" s="133"/>
+      <c r="C48" s="129"/>
       <c r="D48" s="117" t="s">
         <v>127</v>
       </c>
@@ -28453,7 +28453,7 @@
       <c r="B49" s="25" t="s">
         <v>615</v>
       </c>
-      <c r="C49" s="131" t="s">
+      <c r="C49" s="127" t="s">
         <v>955</v>
       </c>
       <c r="D49" s="117" t="s">
@@ -28467,7 +28467,7 @@
       <c r="B50" s="25" t="s">
         <v>617</v>
       </c>
-      <c r="C50" s="132"/>
+      <c r="C50" s="128"/>
       <c r="D50" s="117" t="s">
         <v>127</v>
       </c>
@@ -28479,7 +28479,7 @@
       <c r="B51" s="25" t="s">
         <v>620</v>
       </c>
-      <c r="C51" s="133"/>
+      <c r="C51" s="129"/>
       <c r="D51" s="117" t="s">
         <v>127</v>
       </c>
@@ -28491,7 +28491,7 @@
       <c r="B52" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="C52" s="128" t="s">
+      <c r="C52" s="124" t="s">
         <v>956</v>
       </c>
       <c r="D52" s="117" t="s">
@@ -28505,7 +28505,7 @@
       <c r="B53" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="C53" s="129"/>
+      <c r="C53" s="125"/>
       <c r="D53" s="117" t="s">
         <v>127</v>
       </c>
@@ -28517,7 +28517,7 @@
       <c r="B54" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="C54" s="129"/>
+      <c r="C54" s="125"/>
       <c r="D54" s="117" t="s">
         <v>127</v>
       </c>
@@ -28529,7 +28529,7 @@
       <c r="B55" s="25" t="s">
         <v>876</v>
       </c>
-      <c r="C55" s="129"/>
+      <c r="C55" s="125"/>
       <c r="D55" s="117" t="s">
         <v>127</v>
       </c>
@@ -28541,7 +28541,7 @@
       <c r="B56" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="C56" s="129"/>
+      <c r="C56" s="125"/>
       <c r="D56" s="117" t="s">
         <v>127</v>
       </c>
@@ -28553,7 +28553,7 @@
       <c r="B57" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="C57" s="130"/>
+      <c r="C57" s="126"/>
       <c r="D57" s="117" t="s">
         <v>127</v>
       </c>
@@ -28565,7 +28565,7 @@
       <c r="B58" s="25" t="s">
         <v>428</v>
       </c>
-      <c r="C58" s="134" t="s">
+      <c r="C58" s="130" t="s">
         <v>957</v>
       </c>
       <c r="D58" s="117" t="s">
@@ -28579,7 +28579,7 @@
       <c r="B59" s="25" t="s">
         <v>430</v>
       </c>
-      <c r="C59" s="135"/>
+      <c r="C59" s="131"/>
       <c r="D59" s="117" t="s">
         <v>127</v>
       </c>
@@ -28591,7 +28591,7 @@
       <c r="B60" s="25" t="s">
         <v>438</v>
       </c>
-      <c r="C60" s="135"/>
+      <c r="C60" s="131"/>
       <c r="D60" s="117" t="s">
         <v>127</v>
       </c>
@@ -28603,7 +28603,7 @@
       <c r="B61" s="25" t="s">
         <v>446</v>
       </c>
-      <c r="C61" s="135"/>
+      <c r="C61" s="131"/>
       <c r="D61" s="117" t="s">
         <v>127</v>
       </c>
@@ -28615,7 +28615,7 @@
       <c r="B62" s="25" t="s">
         <v>449</v>
       </c>
-      <c r="C62" s="135"/>
+      <c r="C62" s="131"/>
       <c r="D62" s="117" t="s">
         <v>127</v>
       </c>
@@ -28627,7 +28627,7 @@
       <c r="B63" s="25" t="s">
         <v>452</v>
       </c>
-      <c r="C63" s="135"/>
+      <c r="C63" s="131"/>
       <c r="D63" s="117" t="s">
         <v>127</v>
       </c>
@@ -28639,7 +28639,7 @@
       <c r="B64" s="25" t="s">
         <v>454</v>
       </c>
-      <c r="C64" s="135"/>
+      <c r="C64" s="131"/>
       <c r="D64" s="117" t="s">
         <v>127</v>
       </c>
@@ -28651,7 +28651,7 @@
       <c r="B65" s="25" t="s">
         <v>458</v>
       </c>
-      <c r="C65" s="136"/>
+      <c r="C65" s="132"/>
       <c r="D65" s="117" t="s">
         <v>127</v>
       </c>
@@ -28663,7 +28663,7 @@
       <c r="B66" s="25" t="s">
         <v>892</v>
       </c>
-      <c r="C66" s="126" t="s">
+      <c r="C66" s="133" t="s">
         <v>881</v>
       </c>
       <c r="D66" s="117" t="s">
@@ -28677,7 +28677,7 @@
       <c r="B67" s="25" t="s">
         <v>893</v>
       </c>
-      <c r="C67" s="126"/>
+      <c r="C67" s="133"/>
       <c r="D67" s="117" t="s">
         <v>127</v>
       </c>
@@ -28803,7 +28803,7 @@
       <c r="B77" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="C77" s="126" t="s">
+      <c r="C77" s="133" t="s">
         <v>883</v>
       </c>
       <c r="D77" s="117" t="s">
@@ -28817,7 +28817,7 @@
       <c r="B78" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="C78" s="126"/>
+      <c r="C78" s="133"/>
       <c r="D78" s="117" t="s">
         <v>127</v>
       </c>
@@ -28843,7 +28843,7 @@
       <c r="B80" s="25" t="s">
         <v>532</v>
       </c>
-      <c r="C80" s="126" t="s">
+      <c r="C80" s="133" t="s">
         <v>885</v>
       </c>
       <c r="D80" s="117" t="s">
@@ -28857,7 +28857,7 @@
       <c r="B81" s="25" t="s">
         <v>534</v>
       </c>
-      <c r="C81" s="126"/>
+      <c r="C81" s="133"/>
       <c r="D81" s="117" t="s">
         <v>127</v>
       </c>
@@ -28869,7 +28869,7 @@
       <c r="B82" s="25" t="s">
         <v>537</v>
       </c>
-      <c r="C82" s="126"/>
+      <c r="C82" s="133"/>
       <c r="D82" s="117" t="s">
         <v>127</v>
       </c>
@@ -28881,7 +28881,7 @@
       <c r="B83" s="25" t="s">
         <v>737</v>
       </c>
-      <c r="C83" s="126" t="s">
+      <c r="C83" s="133" t="s">
         <v>886</v>
       </c>
       <c r="D83" s="117" t="s">
@@ -28895,7 +28895,7 @@
       <c r="B84" s="25" t="s">
         <v>744</v>
       </c>
-      <c r="C84" s="126"/>
+      <c r="C84" s="133"/>
       <c r="D84" s="117" t="s">
         <v>127</v>
       </c>
@@ -28907,7 +28907,7 @@
       <c r="B85" s="25" t="s">
         <v>746</v>
       </c>
-      <c r="C85" s="126"/>
+      <c r="C85" s="133"/>
       <c r="D85" s="117" t="s">
         <v>127</v>
       </c>
@@ -28919,7 +28919,7 @@
       <c r="B86" s="25" t="s">
         <v>748</v>
       </c>
-      <c r="C86" s="126"/>
+      <c r="C86" s="133"/>
       <c r="D86" s="117" t="s">
         <v>127</v>
       </c>
@@ -28931,7 +28931,7 @@
       <c r="B87" s="25" t="s">
         <v>750</v>
       </c>
-      <c r="C87" s="126"/>
+      <c r="C87" s="133"/>
       <c r="D87" s="117" t="s">
         <v>127</v>
       </c>
@@ -28943,7 +28943,7 @@
       <c r="B88" s="25" t="s">
         <v>720</v>
       </c>
-      <c r="C88" s="126" t="s">
+      <c r="C88" s="133" t="s">
         <v>887</v>
       </c>
       <c r="D88" s="117" t="s">
@@ -28957,7 +28957,7 @@
       <c r="B89" s="25" t="s">
         <v>722</v>
       </c>
-      <c r="C89" s="126"/>
+      <c r="C89" s="133"/>
       <c r="D89" s="117" t="s">
         <v>127</v>
       </c>
@@ -29782,19 +29782,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="C90:C93"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="C15:C19"/>
-    <mergeCell ref="C20:C25"/>
-    <mergeCell ref="C26:C31"/>
-    <mergeCell ref="C32:C36"/>
-    <mergeCell ref="C37:C48"/>
-    <mergeCell ref="C49:C51"/>
-    <mergeCell ref="C52:C57"/>
-    <mergeCell ref="C58:C65"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="C68:C70"/>
-    <mergeCell ref="C71:C75"/>
     <mergeCell ref="C153:C155"/>
     <mergeCell ref="C2:C11"/>
     <mergeCell ref="C119:C122"/>
@@ -29811,6 +29798,19 @@
     <mergeCell ref="C80:C82"/>
     <mergeCell ref="C83:C87"/>
     <mergeCell ref="C88:C89"/>
+    <mergeCell ref="C90:C93"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="C15:C19"/>
+    <mergeCell ref="C20:C25"/>
+    <mergeCell ref="C26:C31"/>
+    <mergeCell ref="C32:C36"/>
+    <mergeCell ref="C37:C48"/>
+    <mergeCell ref="C49:C51"/>
+    <mergeCell ref="C52:C57"/>
+    <mergeCell ref="C58:C65"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="C68:C70"/>
+    <mergeCell ref="C71:C75"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:B1048576 C1:C2 C12:C1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="4"/>

</xml_diff>